<commit_message>
Update reference file: Y5_B2526_General_&_Special_Surgery_2_B1_reference_data.xlsx
</commit_message>
<xml_diff>
--- a/reference_data/Y5_B2526_General_&_Special_Surgery_2_B1_reference_data.xlsx
+++ b/reference_data/Y5_B2526_General_&_Special_Surgery_2_B1_reference_data.xlsx
@@ -1,13 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -26,7 +25,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <family val="2"/>
       <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b val="1"/>
@@ -66,10 +70,19 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -91,7 +104,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -456,7 +469,7 @@
   </sheetPr>
   <dimension ref="A1:E335"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -499,10 +512,14 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>210768</t>
-        </is>
-      </c>
-      <c r="B2" s="3" t="inlineStr"/>
+          <t>211326</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>سما احمد سعيد النشار</t>
+        </is>
+      </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
           <t>Year 5</t>
@@ -510,7 +527,7 @@
       </c>
       <c r="D2" s="3" t="inlineStr">
         <is>
-          <t>A1</t>
+          <t>B1-1</t>
         </is>
       </c>
       <c r="E2" s="3" t="inlineStr">
@@ -522,10 +539,14 @@
     <row r="3">
       <c r="A3" s="4" t="inlineStr">
         <is>
-          <t>211262</t>
-        </is>
-      </c>
-      <c r="B3" s="4" t="inlineStr"/>
+          <t>211331</t>
+        </is>
+      </c>
+      <c r="B3" s="4" t="inlineStr">
+        <is>
+          <t>ساره وائل محمد عواد العزالى</t>
+        </is>
+      </c>
       <c r="C3" s="4" t="inlineStr">
         <is>
           <t>Year 5</t>
@@ -533,7 +554,7 @@
       </c>
       <c r="D3" s="4" t="inlineStr">
         <is>
-          <t>A1</t>
+          <t>B1-1</t>
         </is>
       </c>
       <c r="E3" s="4" t="inlineStr">
@@ -545,10 +566,14 @@
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>211364</t>
-        </is>
-      </c>
-      <c r="B4" s="3" t="inlineStr"/>
+          <t>211332</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>مها ياسر عبد العظيم محاريق</t>
+        </is>
+      </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
           <t>Year 5</t>
@@ -556,7 +581,7 @@
       </c>
       <c r="D4" s="3" t="inlineStr">
         <is>
-          <t>A1</t>
+          <t>B1-1</t>
         </is>
       </c>
       <c r="E4" s="3" t="inlineStr">
@@ -568,10 +593,14 @@
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>211433</t>
-        </is>
-      </c>
-      <c r="B5" s="4" t="inlineStr"/>
+          <t>211334</t>
+        </is>
+      </c>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>روان محمد عبد العزيز محمد</t>
+        </is>
+      </c>
       <c r="C5" s="4" t="inlineStr">
         <is>
           <t>Year 5</t>
@@ -579,7 +608,7 @@
       </c>
       <c r="D5" s="4" t="inlineStr">
         <is>
-          <t>A1</t>
+          <t>B1-1</t>
         </is>
       </c>
       <c r="E5" s="4" t="inlineStr">
@@ -591,10 +620,14 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>211455</t>
-        </is>
-      </c>
-      <c r="B6" s="3" t="inlineStr"/>
+          <t>211335</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">روان حاتم عبد المنعم احمد </t>
+        </is>
+      </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
           <t>Year 5</t>
@@ -602,7 +635,7 @@
       </c>
       <c r="D6" s="3" t="inlineStr">
         <is>
-          <t>A1</t>
+          <t>B1-1</t>
         </is>
       </c>
       <c r="E6" s="3" t="inlineStr">
@@ -614,10 +647,14 @@
     <row r="7">
       <c r="A7" s="4" t="inlineStr">
         <is>
-          <t>211536</t>
-        </is>
-      </c>
-      <c r="B7" s="4" t="inlineStr"/>
+          <t>211336</t>
+        </is>
+      </c>
+      <c r="B7" s="4" t="inlineStr">
+        <is>
+          <t>امنيه محمد عبد المعز جابر خليل</t>
+        </is>
+      </c>
       <c r="C7" s="4" t="inlineStr">
         <is>
           <t>Year 5</t>
@@ -625,7 +662,7 @@
       </c>
       <c r="D7" s="4" t="inlineStr">
         <is>
-          <t>A1</t>
+          <t>B1-1</t>
         </is>
       </c>
       <c r="E7" s="4" t="inlineStr">
@@ -637,10 +674,14 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>211609</t>
-        </is>
-      </c>
-      <c r="B8" s="3" t="inlineStr"/>
+          <t>211338</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>سلمى محمد محمود عبد الجليل رضوان</t>
+        </is>
+      </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
           <t>Year 5</t>
@@ -648,7 +689,7 @@
       </c>
       <c r="D8" s="3" t="inlineStr">
         <is>
-          <t>A1</t>
+          <t>B1-1</t>
         </is>
       </c>
       <c r="E8" s="3" t="inlineStr">
@@ -660,10 +701,14 @@
     <row r="9">
       <c r="A9" s="4" t="inlineStr">
         <is>
-          <t>211721</t>
-        </is>
-      </c>
-      <c r="B9" s="4" t="inlineStr"/>
+          <t>211341</t>
+        </is>
+      </c>
+      <c r="B9" s="4" t="inlineStr">
+        <is>
+          <t>كريم محمود عبد الله يوسف السيد</t>
+        </is>
+      </c>
       <c r="C9" s="4" t="inlineStr">
         <is>
           <t>Year 5</t>
@@ -671,7 +716,7 @@
       </c>
       <c r="D9" s="4" t="inlineStr">
         <is>
-          <t>A1</t>
+          <t>B1-1</t>
         </is>
       </c>
       <c r="E9" s="4" t="inlineStr">
@@ -683,10 +728,14 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>211833</t>
-        </is>
-      </c>
-      <c r="B10" s="3" t="inlineStr"/>
+          <t>211342</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>احمد مجدى السيد محمد</t>
+        </is>
+      </c>
       <c r="C10" s="3" t="inlineStr">
         <is>
           <t>Year 5</t>
@@ -694,7 +743,7 @@
       </c>
       <c r="D10" s="3" t="inlineStr">
         <is>
-          <t>A1</t>
+          <t>B1-1</t>
         </is>
       </c>
       <c r="E10" s="3" t="inlineStr">
@@ -706,10 +755,14 @@
     <row r="11">
       <c r="A11" s="4" t="inlineStr">
         <is>
-          <t>211948</t>
-        </is>
-      </c>
-      <c r="B11" s="4" t="inlineStr"/>
+          <t>211343</t>
+        </is>
+      </c>
+      <c r="B11" s="4" t="inlineStr">
+        <is>
+          <t>مصطفى صابر عبد الله محمد السيد حسانين</t>
+        </is>
+      </c>
       <c r="C11" s="4" t="inlineStr">
         <is>
           <t>Year 5</t>
@@ -717,7 +770,7 @@
       </c>
       <c r="D11" s="4" t="inlineStr">
         <is>
-          <t>A1</t>
+          <t>B1-1</t>
         </is>
       </c>
       <c r="E11" s="4" t="inlineStr">
@@ -729,10 +782,14 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>212027</t>
-        </is>
-      </c>
-      <c r="B12" s="3" t="inlineStr"/>
+          <t>211345</t>
+        </is>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>حمزه شريف سيد محمد</t>
+        </is>
+      </c>
       <c r="C12" s="3" t="inlineStr">
         <is>
           <t>Year 5</t>
@@ -740,7 +797,7 @@
       </c>
       <c r="D12" s="3" t="inlineStr">
         <is>
-          <t>A1</t>
+          <t>B1-1</t>
         </is>
       </c>
       <c r="E12" s="3" t="inlineStr">
@@ -752,12 +809,12 @@
     <row r="13">
       <c r="A13" s="4" t="inlineStr">
         <is>
-          <t>211326</t>
+          <t>211346</t>
         </is>
       </c>
       <c r="B13" s="4" t="inlineStr">
         <is>
-          <t>سما احمد سعيد النشار</t>
+          <t>يوسف محمد بهاء الدين فوده</t>
         </is>
       </c>
       <c r="C13" s="4" t="inlineStr">
@@ -779,12 +836,12 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>211331</t>
+          <t>211347</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>ساره وائل محمد عواد العزالى</t>
+          <t>مصطفى احمد محمد رجاء ابو عوف</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
@@ -806,12 +863,12 @@
     <row r="15">
       <c r="A15" s="4" t="inlineStr">
         <is>
-          <t>211332</t>
+          <t>211349</t>
         </is>
       </c>
       <c r="B15" s="4" t="inlineStr">
         <is>
-          <t>مها ياسر عبد العظيم محاريق</t>
+          <t>نور محمد كمال محمد رشاد المصرى</t>
         </is>
       </c>
       <c r="C15" s="4" t="inlineStr">
@@ -833,12 +890,12 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>211334</t>
+          <t>211350</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>روان محمد عبد العزيز محمد</t>
+          <t>توماس هانى عبدالنعيم ملك</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
@@ -860,12 +917,12 @@
     <row r="17">
       <c r="A17" s="4" t="inlineStr">
         <is>
-          <t>211335</t>
+          <t>211352</t>
         </is>
       </c>
       <c r="B17" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">روان حاتم عبد المنعم احمد </t>
+          <t>عبد الله احمد عباس احمد الزنكلونى</t>
         </is>
       </c>
       <c r="C17" s="4" t="inlineStr">
@@ -887,12 +944,12 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>211336</t>
+          <t>211355</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>امنيه محمد عبد المعز جابر خليل</t>
+          <t xml:space="preserve">ميرولا ميكل مقبل عزمى </t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
@@ -914,12 +971,12 @@
     <row r="19">
       <c r="A19" s="4" t="inlineStr">
         <is>
-          <t>211338</t>
+          <t>211357</t>
         </is>
       </c>
       <c r="B19" s="4" t="inlineStr">
         <is>
-          <t>سلمى محمد محمود عبد الجليل رضوان</t>
+          <t>اسماعيل فهد احمد فضل</t>
         </is>
       </c>
       <c r="C19" s="4" t="inlineStr">
@@ -941,12 +998,12 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>211341</t>
+          <t>211359</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>كريم محمود عبد الله يوسف السيد</t>
+          <t>نور الدين حازم احمد عبد العزيز</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
@@ -968,12 +1025,12 @@
     <row r="21">
       <c r="A21" s="4" t="inlineStr">
         <is>
-          <t>211342</t>
+          <t>211361</t>
         </is>
       </c>
       <c r="B21" s="4" t="inlineStr">
         <is>
-          <t>احمد مجدى السيد محمد</t>
+          <t>اسر وليد فوزى محمد</t>
         </is>
       </c>
       <c r="C21" s="4" t="inlineStr">
@@ -995,12 +1052,12 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>211343</t>
+          <t>211363</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
         <is>
-          <t>مصطفى صابر عبد الله محمد السيد حسانين</t>
+          <t>مارك مينا يونان ميخائيل</t>
         </is>
       </c>
       <c r="C22" s="3" t="inlineStr">
@@ -1022,12 +1079,12 @@
     <row r="23">
       <c r="A23" s="4" t="inlineStr">
         <is>
-          <t>211345</t>
+          <t>211365</t>
         </is>
       </c>
       <c r="B23" s="4" t="inlineStr">
         <is>
-          <t>حمزه شريف سيد محمد</t>
+          <t>عادل عمرو عادل عبد العال حسن</t>
         </is>
       </c>
       <c r="C23" s="4" t="inlineStr">
@@ -1049,12 +1106,12 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>211346</t>
+          <t>211366</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
         <is>
-          <t>يوسف محمد بهاء الدين فوده</t>
+          <t>منه الله محمود عمر بكر حباكه</t>
         </is>
       </c>
       <c r="C24" s="3" t="inlineStr">
@@ -1076,12 +1133,12 @@
     <row r="25">
       <c r="A25" s="4" t="inlineStr">
         <is>
-          <t>211347</t>
+          <t>211368</t>
         </is>
       </c>
       <c r="B25" s="4" t="inlineStr">
         <is>
-          <t>مصطفى احمد محمد رجاء ابو عوف</t>
+          <t>يوسف حسام الدين حمدى السعيد متولى</t>
         </is>
       </c>
       <c r="C25" s="4" t="inlineStr">
@@ -1103,12 +1160,12 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>211349</t>
+          <t>211369</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t>نور محمد كمال محمد رشاد المصرى</t>
+          <t>اميره معتز محمود محمد ابراهيم</t>
         </is>
       </c>
       <c r="C26" s="3" t="inlineStr">
@@ -1130,12 +1187,12 @@
     <row r="27">
       <c r="A27" s="4" t="inlineStr">
         <is>
-          <t>211350</t>
+          <t>211370</t>
         </is>
       </c>
       <c r="B27" s="4" t="inlineStr">
         <is>
-          <t>توماس هانى عبدالنعيم ملك</t>
+          <t>سيف الدين ناصر احمد عبد النظير</t>
         </is>
       </c>
       <c r="C27" s="4" t="inlineStr">
@@ -1157,12 +1214,12 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>211352</t>
+          <t>210872</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
         <is>
-          <t>عبد الله احمد عباس احمد الزنكلونى</t>
+          <t>قيس شعبان محمد عون</t>
         </is>
       </c>
       <c r="C28" s="3" t="inlineStr">
@@ -1172,7 +1229,7 @@
       </c>
       <c r="D28" s="3" t="inlineStr">
         <is>
-          <t>B1-1</t>
+          <t>B1-10</t>
         </is>
       </c>
       <c r="E28" s="3" t="inlineStr">
@@ -1184,12 +1241,12 @@
     <row r="29">
       <c r="A29" s="4" t="inlineStr">
         <is>
-          <t>211355</t>
+          <t>211930</t>
         </is>
       </c>
       <c r="B29" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">ميرولا ميكل مقبل عزمى </t>
+          <t>عبد الرحمن محمد ابراهيم عبد الرازق القناوى</t>
         </is>
       </c>
       <c r="C29" s="4" t="inlineStr">
@@ -1199,7 +1256,7 @@
       </c>
       <c r="D29" s="4" t="inlineStr">
         <is>
-          <t>B1-1</t>
+          <t>B1-10</t>
         </is>
       </c>
       <c r="E29" s="4" t="inlineStr">
@@ -1211,12 +1268,12 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>211357</t>
+          <t>211931</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
         <is>
-          <t>اسماعيل فهد احمد فضل</t>
+          <t>ابى ماجد مصطفى مصطفى</t>
         </is>
       </c>
       <c r="C30" s="3" t="inlineStr">
@@ -1226,7 +1283,7 @@
       </c>
       <c r="D30" s="3" t="inlineStr">
         <is>
-          <t>B1-1</t>
+          <t>B1-10</t>
         </is>
       </c>
       <c r="E30" s="3" t="inlineStr">
@@ -1238,12 +1295,12 @@
     <row r="31">
       <c r="A31" s="4" t="inlineStr">
         <is>
-          <t>211359</t>
+          <t>211940</t>
         </is>
       </c>
       <c r="B31" s="4" t="inlineStr">
         <is>
-          <t>نور الدين حازم احمد عبد العزيز</t>
+          <t>ماب محمد رجب الضبع</t>
         </is>
       </c>
       <c r="C31" s="4" t="inlineStr">
@@ -1253,7 +1310,7 @@
       </c>
       <c r="D31" s="4" t="inlineStr">
         <is>
-          <t>B1-1</t>
+          <t>B1-10</t>
         </is>
       </c>
       <c r="E31" s="4" t="inlineStr">
@@ -1265,12 +1322,12 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>211361</t>
+          <t>211942</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
         <is>
-          <t>اسر وليد فوزى محمد</t>
+          <t>اسامه محمد جبريل محمد</t>
         </is>
       </c>
       <c r="C32" s="3" t="inlineStr">
@@ -1280,7 +1337,7 @@
       </c>
       <c r="D32" s="3" t="inlineStr">
         <is>
-          <t>B1-1</t>
+          <t>B1-10</t>
         </is>
       </c>
       <c r="E32" s="3" t="inlineStr">
@@ -1292,12 +1349,12 @@
     <row r="33">
       <c r="A33" s="4" t="inlineStr">
         <is>
-          <t>211363</t>
+          <t>211943</t>
         </is>
       </c>
       <c r="B33" s="4" t="inlineStr">
         <is>
-          <t>مارك مينا يونان ميخائيل</t>
+          <t>مريم طارق تيمور توفيق</t>
         </is>
       </c>
       <c r="C33" s="4" t="inlineStr">
@@ -1307,7 +1364,7 @@
       </c>
       <c r="D33" s="4" t="inlineStr">
         <is>
-          <t>B1-1</t>
+          <t>B1-10</t>
         </is>
       </c>
       <c r="E33" s="4" t="inlineStr">
@@ -1319,12 +1376,12 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>211365</t>
+          <t>211945</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
         <is>
-          <t>عادل عمرو عادل عبد العال حسن</t>
+          <t>محمد جهاد عبد الهادى مشعل</t>
         </is>
       </c>
       <c r="C34" s="3" t="inlineStr">
@@ -1334,7 +1391,7 @@
       </c>
       <c r="D34" s="3" t="inlineStr">
         <is>
-          <t>B1-1</t>
+          <t>B1-10</t>
         </is>
       </c>
       <c r="E34" s="3" t="inlineStr">
@@ -1346,12 +1403,12 @@
     <row r="35">
       <c r="A35" s="4" t="inlineStr">
         <is>
-          <t>211366</t>
+          <t>211946</t>
         </is>
       </c>
       <c r="B35" s="4" t="inlineStr">
         <is>
-          <t>منه الله محمود عمر بكر حباكه</t>
+          <t>نسيبه فرج على بازاما</t>
         </is>
       </c>
       <c r="C35" s="4" t="inlineStr">
@@ -1361,7 +1418,7 @@
       </c>
       <c r="D35" s="4" t="inlineStr">
         <is>
-          <t>B1-1</t>
+          <t>B1-10</t>
         </is>
       </c>
       <c r="E35" s="4" t="inlineStr">
@@ -1373,12 +1430,12 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>211368</t>
+          <t>211948</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
         <is>
-          <t>يوسف حسام الدين حمدى السعيد متولى</t>
+          <t>معمر مفتاح سعد مفتاح</t>
         </is>
       </c>
       <c r="C36" s="3" t="inlineStr">
@@ -1388,7 +1445,7 @@
       </c>
       <c r="D36" s="3" t="inlineStr">
         <is>
-          <t>B1-1</t>
+          <t>B1-10</t>
         </is>
       </c>
       <c r="E36" s="3" t="inlineStr">
@@ -1400,12 +1457,12 @@
     <row r="37">
       <c r="A37" s="4" t="inlineStr">
         <is>
-          <t>211369</t>
+          <t>211955</t>
         </is>
       </c>
       <c r="B37" s="4" t="inlineStr">
         <is>
-          <t>اميره معتز محمود محمد ابراهيم</t>
+          <t>راما عبد الله خوام</t>
         </is>
       </c>
       <c r="C37" s="4" t="inlineStr">
@@ -1415,7 +1472,7 @@
       </c>
       <c r="D37" s="4" t="inlineStr">
         <is>
-          <t>B1-1</t>
+          <t>B1-10</t>
         </is>
       </c>
       <c r="E37" s="4" t="inlineStr">
@@ -1427,12 +1484,12 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>211370</t>
+          <t>211957</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
         <is>
-          <t>سيف الدين ناصر احمد عبد النظير</t>
+          <t>يحيى طعان نافع السعايده</t>
         </is>
       </c>
       <c r="C38" s="3" t="inlineStr">
@@ -1442,7 +1499,7 @@
       </c>
       <c r="D38" s="3" t="inlineStr">
         <is>
-          <t>B1-1</t>
+          <t>B1-10</t>
         </is>
       </c>
       <c r="E38" s="3" t="inlineStr">
@@ -1454,12 +1511,12 @@
     <row r="39">
       <c r="A39" s="4" t="inlineStr">
         <is>
-          <t>201820</t>
+          <t>211958</t>
         </is>
       </c>
       <c r="B39" s="4" t="inlineStr">
         <is>
-          <t>تميم بدر حسين</t>
+          <t>راويه معاذ عمر ماشطه</t>
         </is>
       </c>
       <c r="C39" s="4" t="inlineStr">
@@ -1481,12 +1538,12 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>210033</t>
+          <t>211968</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
         <is>
-          <t>محمود مهدى حربى ابو هدوان</t>
+          <t>اسامه عبدالله علي فرحان</t>
         </is>
       </c>
       <c r="C40" s="3" t="inlineStr">
@@ -1508,12 +1565,12 @@
     <row r="41">
       <c r="A41" s="4" t="inlineStr">
         <is>
-          <t>210729</t>
+          <t>211969</t>
         </is>
       </c>
       <c r="B41" s="4" t="inlineStr">
         <is>
-          <t>سراج مصطفى محمد ابو لقمه</t>
+          <t>مصطفى توفيق خلف</t>
         </is>
       </c>
       <c r="C41" s="4" t="inlineStr">
@@ -1535,12 +1592,12 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>210735</t>
+          <t>211974</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
         <is>
-          <t>محمد فرج على القمودى</t>
+          <t>سلمى محمد ذهنى شحاته</t>
         </is>
       </c>
       <c r="C42" s="3" t="inlineStr">
@@ -1562,12 +1619,12 @@
     <row r="43">
       <c r="A43" s="4" t="inlineStr">
         <is>
-          <t>211925</t>
+          <t>211975</t>
         </is>
       </c>
       <c r="B43" s="4" t="inlineStr">
         <is>
-          <t>حسن ايمن الحريرى</t>
+          <t>هدى مجددى</t>
         </is>
       </c>
       <c r="C43" s="4" t="inlineStr">
@@ -1589,12 +1646,12 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>211955</t>
+          <t>211977</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
         <is>
-          <t>قيس شعبان محمد عون</t>
+          <t>دعاء بدر الدين جعفر عثمان</t>
         </is>
       </c>
       <c r="C44" s="3" t="inlineStr">
@@ -1616,12 +1673,12 @@
     <row r="45">
       <c r="A45" s="4" t="inlineStr">
         <is>
-          <t>211957</t>
+          <t>211981</t>
         </is>
       </c>
       <c r="B45" s="4" t="inlineStr">
         <is>
-          <t>عبد الرحمن محمد ابراهيم عبد الرازق القناوى</t>
+          <t>هيا محمد عماد قارى</t>
         </is>
       </c>
       <c r="C45" s="4" t="inlineStr">
@@ -1643,12 +1700,12 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>211958</t>
+          <t>211982</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
         <is>
-          <t>ابى ماجد مصطفى مصطفى</t>
+          <t>محمد على عيسى</t>
         </is>
       </c>
       <c r="C46" s="3" t="inlineStr">
@@ -1670,12 +1727,12 @@
     <row r="47">
       <c r="A47" s="4" t="inlineStr">
         <is>
-          <t>211968</t>
+          <t>211988</t>
         </is>
       </c>
       <c r="B47" s="4" t="inlineStr">
         <is>
-          <t>ماب محمد رجب الضبع</t>
+          <t>محمد سمير حموده شعت</t>
         </is>
       </c>
       <c r="C47" s="4" t="inlineStr">
@@ -1697,12 +1754,12 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>211969</t>
+          <t>211989</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
         <is>
-          <t>اسامه محمد جبريل محمد</t>
+          <t>حازم كمال محمد سعيد</t>
         </is>
       </c>
       <c r="C48" s="3" t="inlineStr">
@@ -1724,12 +1781,12 @@
     <row r="49">
       <c r="A49" s="4" t="inlineStr">
         <is>
-          <t>211974</t>
+          <t>211991</t>
         </is>
       </c>
       <c r="B49" s="4" t="inlineStr">
         <is>
-          <t>مريم طارق تيمور توفيق</t>
+          <t>مؤيد سامى توفيق ابو ريده</t>
         </is>
       </c>
       <c r="C49" s="4" t="inlineStr">
@@ -1751,12 +1808,12 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>211975</t>
+          <t>211995</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
         <is>
-          <t>محمد جهاد عبد الهادى مشعل</t>
+          <t>تميم بدر حسين</t>
         </is>
       </c>
       <c r="C50" s="3" t="inlineStr">
@@ -1778,12 +1835,12 @@
     <row r="51">
       <c r="A51" s="4" t="inlineStr">
         <is>
-          <t>211977</t>
+          <t>211997</t>
         </is>
       </c>
       <c r="B51" s="4" t="inlineStr">
         <is>
-          <t>نسيبه فرج على بازاما</t>
+          <t>محمود مهدى حربى ابو هدوان</t>
         </is>
       </c>
       <c r="C51" s="4" t="inlineStr">
@@ -1805,12 +1862,12 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>211981</t>
+          <t>212003</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
         <is>
-          <t>معمر مفتاح سعد مفتاح</t>
+          <t>سراج مصطفى محمد ابو لقمه</t>
         </is>
       </c>
       <c r="C52" s="3" t="inlineStr">
@@ -1832,12 +1889,12 @@
     <row r="53">
       <c r="A53" s="4" t="inlineStr">
         <is>
-          <t>211982</t>
+          <t>212004</t>
         </is>
       </c>
       <c r="B53" s="4" t="inlineStr">
         <is>
-          <t>راما عبد الله خوام</t>
+          <t>محمد فرج على القمودى</t>
         </is>
       </c>
       <c r="C53" s="4" t="inlineStr">
@@ -1859,12 +1916,12 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>211988</t>
+          <t>212010</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
         <is>
-          <t>يحيى طعان نافع السعايده</t>
+          <t>حسن ايمن الحريرى</t>
         </is>
       </c>
       <c r="C54" s="3" t="inlineStr">
@@ -1886,12 +1943,12 @@
     <row r="55">
       <c r="A55" s="4" t="inlineStr">
         <is>
-          <t>211989</t>
+          <t>212026</t>
         </is>
       </c>
       <c r="B55" s="4" t="inlineStr">
         <is>
-          <t>راويه معاذ عمر ماشطه</t>
+          <t>عبد الله عماد المثقال</t>
         </is>
       </c>
       <c r="C55" s="4" t="inlineStr">
@@ -1913,12 +1970,12 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>211991</t>
+          <t>212030</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
         <is>
-          <t>اسامه عبدالله علي فرحان</t>
+          <t>المعتصم محمود عمر عمر</t>
         </is>
       </c>
       <c r="C56" s="3" t="inlineStr">
@@ -1940,12 +1997,12 @@
     <row r="57">
       <c r="A57" s="4" t="inlineStr">
         <is>
-          <t>211995</t>
+          <t>212057</t>
         </is>
       </c>
       <c r="B57" s="4" t="inlineStr">
         <is>
-          <t>مصطفى توفيق خلف</t>
+          <t>صلاح الدين رياض الناصير</t>
         </is>
       </c>
       <c r="C57" s="4" t="inlineStr">
@@ -1967,12 +2024,12 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>211997</t>
+          <t>212087</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
         <is>
-          <t>سلمى محمد ذهنى شحاته</t>
+          <t>محمد رافد محمد</t>
         </is>
       </c>
       <c r="C58" s="3" t="inlineStr">
@@ -1994,12 +2051,12 @@
     <row r="59">
       <c r="A59" s="4" t="inlineStr">
         <is>
-          <t>212003</t>
+          <t>201820</t>
         </is>
       </c>
       <c r="B59" s="4" t="inlineStr">
         <is>
-          <t>هدى مجددى</t>
+          <t>محمد سعيد احمد</t>
         </is>
       </c>
       <c r="C59" s="4" t="inlineStr">
@@ -2009,7 +2066,7 @@
       </c>
       <c r="D59" s="4" t="inlineStr">
         <is>
-          <t>B1-10</t>
+          <t>B1-11</t>
         </is>
       </c>
       <c r="E59" s="4" t="inlineStr">
@@ -2021,12 +2078,12 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>212004</t>
+          <t>210033</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
         <is>
-          <t>دعاء بدر الدين جعفر عثمان</t>
+          <t>هنا محمد عبد المنعم محمد</t>
         </is>
       </c>
       <c r="C60" s="3" t="inlineStr">
@@ -2036,7 +2093,7 @@
       </c>
       <c r="D60" s="3" t="inlineStr">
         <is>
-          <t>B1-10</t>
+          <t>B1-11</t>
         </is>
       </c>
       <c r="E60" s="3" t="inlineStr">
@@ -2048,12 +2105,12 @@
     <row r="61">
       <c r="A61" s="4" t="inlineStr">
         <is>
-          <t>212010</t>
+          <t>210729</t>
         </is>
       </c>
       <c r="B61" s="4" t="inlineStr">
         <is>
-          <t>هيا محمد عماد قارى</t>
+          <t>ندى رافت عبد الغفار محمد السبع</t>
         </is>
       </c>
       <c r="C61" s="4" t="inlineStr">
@@ -2063,7 +2120,7 @@
       </c>
       <c r="D61" s="4" t="inlineStr">
         <is>
-          <t>B1-10</t>
+          <t>B1-11</t>
         </is>
       </c>
       <c r="E61" s="4" t="inlineStr">
@@ -2075,12 +2132,12 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>212016</t>
+          <t>210735</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
         <is>
-          <t>عبد الله عماد المثقال</t>
+          <t>ندى محمد السيد ابراهيم البلام</t>
         </is>
       </c>
       <c r="C62" s="3" t="inlineStr">
@@ -2090,7 +2147,7 @@
       </c>
       <c r="D62" s="3" t="inlineStr">
         <is>
-          <t>B1-10</t>
+          <t>B1-11</t>
         </is>
       </c>
       <c r="E62" s="3" t="inlineStr">
@@ -2102,12 +2159,12 @@
     <row r="63">
       <c r="A63" s="4" t="inlineStr">
         <is>
-          <t>212019</t>
+          <t>211925</t>
         </is>
       </c>
       <c r="B63" s="4" t="inlineStr">
         <is>
-          <t>المعتصم محمود عمر عمر</t>
+          <t>Ibrahim Nuradin Mahamoud</t>
         </is>
       </c>
       <c r="C63" s="4" t="inlineStr">
@@ -2117,7 +2174,7 @@
       </c>
       <c r="D63" s="4" t="inlineStr">
         <is>
-          <t>B1-10</t>
+          <t>B1-11</t>
         </is>
       </c>
       <c r="E63" s="4" t="inlineStr">
@@ -2129,12 +2186,12 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>212020</t>
+          <t>212016</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
         <is>
-          <t>صلاح الدين رياض الناصير</t>
+          <t>محمد وضاح مشمشان</t>
         </is>
       </c>
       <c r="C64" s="3" t="inlineStr">
@@ -2144,7 +2201,7 @@
       </c>
       <c r="D64" s="3" t="inlineStr">
         <is>
-          <t>B1-10</t>
+          <t>B1-11</t>
         </is>
       </c>
       <c r="E64" s="3" t="inlineStr">
@@ -2156,12 +2213,12 @@
     <row r="65">
       <c r="A65" s="4" t="inlineStr">
         <is>
-          <t>212022</t>
+          <t>212019</t>
         </is>
       </c>
       <c r="B65" s="4" t="inlineStr">
         <is>
-          <t>محمد رافد محمد</t>
+          <t>محمد احمد باسل رضوان</t>
         </is>
       </c>
       <c r="C65" s="4" t="inlineStr">
@@ -2171,7 +2228,7 @@
       </c>
       <c r="D65" s="4" t="inlineStr">
         <is>
-          <t>B1-10</t>
+          <t>B1-11</t>
         </is>
       </c>
       <c r="E65" s="4" t="inlineStr">
@@ -2183,12 +2240,12 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>212026</t>
+          <t>212020</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
         <is>
-          <t>محمد على عيسى</t>
+          <t>احمد محمد سمير الزايغ</t>
         </is>
       </c>
       <c r="C66" s="3" t="inlineStr">
@@ -2198,7 +2255,7 @@
       </c>
       <c r="D66" s="3" t="inlineStr">
         <is>
-          <t>B1-10</t>
+          <t>B1-11</t>
         </is>
       </c>
       <c r="E66" s="3" t="inlineStr">
@@ -2210,12 +2267,12 @@
     <row r="67">
       <c r="A67" s="4" t="inlineStr">
         <is>
-          <t>212030</t>
+          <t>212022</t>
         </is>
       </c>
       <c r="B67" s="4" t="inlineStr">
         <is>
-          <t>محمد سمير حموده شعت</t>
+          <t>اسامه فريد جمال حسونه</t>
         </is>
       </c>
       <c r="C67" s="4" t="inlineStr">
@@ -2225,7 +2282,7 @@
       </c>
       <c r="D67" s="4" t="inlineStr">
         <is>
-          <t>B1-10</t>
+          <t>B1-11</t>
         </is>
       </c>
       <c r="E67" s="4" t="inlineStr">
@@ -2237,12 +2294,12 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>212057</t>
+          <t>212027</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
         <is>
-          <t>حازم كمال محمد سعيد</t>
+          <t>خالد سعد مرى عداى محسن</t>
         </is>
       </c>
       <c r="C68" s="3" t="inlineStr">
@@ -2252,7 +2309,7 @@
       </c>
       <c r="D68" s="3" t="inlineStr">
         <is>
-          <t>B1-10</t>
+          <t>B1-11</t>
         </is>
       </c>
       <c r="E68" s="3" t="inlineStr">
@@ -2264,12 +2321,12 @@
     <row r="69">
       <c r="A69" s="4" t="inlineStr">
         <is>
-          <t>212087</t>
+          <t>212034</t>
         </is>
       </c>
       <c r="B69" s="4" t="inlineStr">
         <is>
-          <t>مؤيد سامى توفيق ابو ريده</t>
+          <t>باسل محمد جميل المومنى</t>
         </is>
       </c>
       <c r="C69" s="4" t="inlineStr">
@@ -2279,7 +2336,7 @@
       </c>
       <c r="D69" s="4" t="inlineStr">
         <is>
-          <t>B1-10</t>
+          <t>B1-11</t>
         </is>
       </c>
       <c r="E69" s="4" t="inlineStr">
@@ -2291,12 +2348,12 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>191084</t>
+          <t>212035</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
         <is>
-          <t>خالد سعد مرى عداى محسن</t>
+          <t>غالب ثائر ابراهيم ابو فرده</t>
         </is>
       </c>
       <c r="C70" s="3" t="inlineStr">
@@ -2318,12 +2375,12 @@
     <row r="71">
       <c r="A71" s="4" t="inlineStr">
         <is>
-          <t>200328</t>
+          <t>212051</t>
         </is>
       </c>
       <c r="B71" s="4" t="inlineStr">
         <is>
-          <t>باسل محمد جميل المومنى</t>
+          <t>عز الدين اسامه المنجد</t>
         </is>
       </c>
       <c r="C71" s="4" t="inlineStr">
@@ -2345,12 +2402,12 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>200346</t>
+          <t>212060</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
         <is>
-          <t>غالب ثائر ابراهيم ابو فرده</t>
+          <t>محمد عثمان ابراهيم تمر</t>
         </is>
       </c>
       <c r="C72" s="3" t="inlineStr">
@@ -2372,12 +2429,12 @@
     <row r="73">
       <c r="A73" s="4" t="inlineStr">
         <is>
-          <t>200732</t>
+          <t>212067</t>
         </is>
       </c>
       <c r="B73" s="4" t="inlineStr">
         <is>
-          <t>عز الدين اسامه المنجد</t>
+          <t>اياس عبد الكريم عزت سرحان</t>
         </is>
       </c>
       <c r="C73" s="4" t="inlineStr">
@@ -2399,12 +2456,12 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>201932</t>
+          <t>212070</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
         <is>
-          <t>محمد عثمان ابراهيم تمر</t>
+          <t>سامى زياد سامى معالى</t>
         </is>
       </c>
       <c r="C74" s="3" t="inlineStr">
@@ -2426,12 +2483,12 @@
     <row r="75">
       <c r="A75" s="4" t="inlineStr">
         <is>
-          <t>202039</t>
+          <t>212074</t>
         </is>
       </c>
       <c r="B75" s="4" t="inlineStr">
         <is>
-          <t>اياس عبد الكريم عزت سرحان</t>
+          <t>Abdulshakur Iman Omar</t>
         </is>
       </c>
       <c r="C75" s="4" t="inlineStr">
@@ -2453,12 +2510,12 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>210423</t>
+          <t>212076</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
         <is>
-          <t>سامى زياد سامى معالى</t>
+          <t>محمود محمد باسل عجيبه</t>
         </is>
       </c>
       <c r="C76" s="3" t="inlineStr">
@@ -2480,12 +2537,12 @@
     <row r="77">
       <c r="A77" s="4" t="inlineStr">
         <is>
-          <t>211045</t>
+          <t>212080</t>
         </is>
       </c>
       <c r="B77" s="4" t="inlineStr">
         <is>
-          <t>Abdulshakur Iman Omar</t>
+          <t>محمد صالح محمد غياث فلاحه</t>
         </is>
       </c>
       <c r="C77" s="4" t="inlineStr">
@@ -2507,12 +2564,12 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>211067</t>
+          <t>191084</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
         <is>
-          <t>محمود محمد باسل عجيبه</t>
+          <t>محمد زين العابدين محمد شاهين</t>
         </is>
       </c>
       <c r="C78" s="3" t="inlineStr">
@@ -2522,7 +2579,7 @@
       </c>
       <c r="D78" s="3" t="inlineStr">
         <is>
-          <t>B1-11</t>
+          <t>B1-12</t>
         </is>
       </c>
       <c r="E78" s="3" t="inlineStr">
@@ -2534,12 +2591,12 @@
     <row r="79">
       <c r="A79" s="4" t="inlineStr">
         <is>
-          <t>211201</t>
+          <t>200328</t>
         </is>
       </c>
       <c r="B79" s="4" t="inlineStr">
         <is>
-          <t>محمد صالح محمد غياث فلاحه</t>
+          <t>سها ابو هيسه احمد ابو هيسه</t>
         </is>
       </c>
       <c r="C79" s="4" t="inlineStr">
@@ -2549,7 +2606,7 @@
       </c>
       <c r="D79" s="4" t="inlineStr">
         <is>
-          <t>B1-11</t>
+          <t>B1-12</t>
         </is>
       </c>
       <c r="E79" s="4" t="inlineStr">
@@ -2561,12 +2618,12 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>212034</t>
+          <t>200346</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
         <is>
-          <t>محمد سعيد احمد</t>
+          <t>شهاب عماد رشاد الفقى</t>
         </is>
       </c>
       <c r="C80" s="3" t="inlineStr">
@@ -2576,7 +2633,7 @@
       </c>
       <c r="D80" s="3" t="inlineStr">
         <is>
-          <t>B1-11</t>
+          <t>B1-12</t>
         </is>
       </c>
       <c r="E80" s="3" t="inlineStr">
@@ -2588,12 +2645,12 @@
     <row r="81">
       <c r="A81" s="4" t="inlineStr">
         <is>
-          <t>212035</t>
+          <t>200732</t>
         </is>
       </c>
       <c r="B81" s="4" t="inlineStr">
         <is>
-          <t>هنا محمد عبد المنعم محمد</t>
+          <t>هنا محمد مصطفى كامل الطويل</t>
         </is>
       </c>
       <c r="C81" s="4" t="inlineStr">
@@ -2603,7 +2660,7 @@
       </c>
       <c r="D81" s="4" t="inlineStr">
         <is>
-          <t>B1-11</t>
+          <t>B1-12</t>
         </is>
       </c>
       <c r="E81" s="4" t="inlineStr">
@@ -2615,12 +2672,12 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>212051</t>
+          <t>201932</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
         <is>
-          <t>ندى رافت عبد الغفار محمد السبع</t>
+          <t>عبد الكريم سليمان حمد</t>
         </is>
       </c>
       <c r="C82" s="3" t="inlineStr">
@@ -2630,7 +2687,7 @@
       </c>
       <c r="D82" s="3" t="inlineStr">
         <is>
-          <t>B1-11</t>
+          <t>B1-12</t>
         </is>
       </c>
       <c r="E82" s="3" t="inlineStr">
@@ -2642,12 +2699,12 @@
     <row r="83">
       <c r="A83" s="4" t="inlineStr">
         <is>
-          <t>212060</t>
+          <t>202039</t>
         </is>
       </c>
       <c r="B83" s="4" t="inlineStr">
         <is>
-          <t>ندى محمد السيد ابراهيم البلام</t>
+          <t>ايهم كريم على</t>
         </is>
       </c>
       <c r="C83" s="4" t="inlineStr">
@@ -2657,7 +2714,7 @@
       </c>
       <c r="D83" s="4" t="inlineStr">
         <is>
-          <t>B1-11</t>
+          <t>B1-12</t>
         </is>
       </c>
       <c r="E83" s="4" t="inlineStr">
@@ -2669,12 +2726,12 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>212067</t>
+          <t>210423</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
         <is>
-          <t>Ibrahim Nuradin Mahamoud</t>
+          <t>ثريا محمد عبد النبي ابراهيم حامد</t>
         </is>
       </c>
       <c r="C84" s="3" t="inlineStr">
@@ -2684,7 +2741,7 @@
       </c>
       <c r="D84" s="3" t="inlineStr">
         <is>
-          <t>B1-11</t>
+          <t>B1-12</t>
         </is>
       </c>
       <c r="E84" s="3" t="inlineStr">
@@ -2696,12 +2753,12 @@
     <row r="85">
       <c r="A85" s="4" t="inlineStr">
         <is>
-          <t>212070</t>
+          <t>211045</t>
         </is>
       </c>
       <c r="B85" s="4" t="inlineStr">
         <is>
-          <t>محمد وضاح مشمشان</t>
+          <t>Hamza Muhumed Dahir</t>
         </is>
       </c>
       <c r="C85" s="4" t="inlineStr">
@@ -2711,7 +2768,7 @@
       </c>
       <c r="D85" s="4" t="inlineStr">
         <is>
-          <t>B1-11</t>
+          <t>B1-12</t>
         </is>
       </c>
       <c r="E85" s="4" t="inlineStr">
@@ -2723,12 +2780,12 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>212074</t>
+          <t>211067</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
         <is>
-          <t>محمد احمد باسل رضوان</t>
+          <t>نوران بنت اشرف بن محمد عثمان</t>
         </is>
       </c>
       <c r="C86" s="3" t="inlineStr">
@@ -2738,7 +2795,7 @@
       </c>
       <c r="D86" s="3" t="inlineStr">
         <is>
-          <t>B1-11</t>
+          <t>B1-12</t>
         </is>
       </c>
       <c r="E86" s="3" t="inlineStr">
@@ -2750,12 +2807,12 @@
     <row r="87">
       <c r="A87" s="4" t="inlineStr">
         <is>
-          <t>212076</t>
+          <t>211201</t>
         </is>
       </c>
       <c r="B87" s="4" t="inlineStr">
         <is>
-          <t>احمد محمد سمير الزايغ</t>
+          <t>الحسن خالد على حزام</t>
         </is>
       </c>
       <c r="C87" s="4" t="inlineStr">
@@ -2765,7 +2822,7 @@
       </c>
       <c r="D87" s="4" t="inlineStr">
         <is>
-          <t>B1-11</t>
+          <t>B1-12</t>
         </is>
       </c>
       <c r="E87" s="4" t="inlineStr">
@@ -2777,12 +2834,12 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>212080</t>
+          <t>211262</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
         <is>
-          <t>اسامه فريد جمال حسونه</t>
+          <t>رغد ابراهيم محمد ابو طير</t>
         </is>
       </c>
       <c r="C88" s="3" t="inlineStr">
@@ -2792,7 +2849,7 @@
       </c>
       <c r="D88" s="3" t="inlineStr">
         <is>
-          <t>B1-11</t>
+          <t>B1-12</t>
         </is>
       </c>
       <c r="E88" s="3" t="inlineStr">
@@ -2809,7 +2866,7 @@
       </c>
       <c r="B89" s="4" t="inlineStr">
         <is>
-          <t>محمد زين العابدين محمد شاهين</t>
+          <t>راكان عبد الحافظ محمد العودات</t>
         </is>
       </c>
       <c r="C89" s="4" t="inlineStr">
@@ -2836,7 +2893,7 @@
       </c>
       <c r="B90" s="3" t="inlineStr">
         <is>
-          <t>سها ابو هيسه احمد ابو هيسه</t>
+          <t>مراء بنت صبرى بن عدنان كلجى</t>
         </is>
       </c>
       <c r="C90" s="3" t="inlineStr">
@@ -2863,7 +2920,7 @@
       </c>
       <c r="B91" s="4" t="inlineStr">
         <is>
-          <t>شهاب عماد رشاد الفقى</t>
+          <t>سجى موسى محمد موسى</t>
         </is>
       </c>
       <c r="C91" s="4" t="inlineStr">
@@ -2890,7 +2947,7 @@
       </c>
       <c r="B92" s="3" t="inlineStr">
         <is>
-          <t>هنا محمد مصطفى كامل الطويل</t>
+          <t>مريم يسرى احمد عثمان محمد</t>
         </is>
       </c>
       <c r="C92" s="3" t="inlineStr">
@@ -2917,7 +2974,7 @@
       </c>
       <c r="B93" s="4" t="inlineStr">
         <is>
-          <t>عبد الكريم سليمان حمد</t>
+          <t xml:space="preserve"> ايه حسين محمد السيد احمد قوره    </t>
         </is>
       </c>
       <c r="C93" s="4" t="inlineStr">
@@ -2944,7 +3001,7 @@
       </c>
       <c r="B94" s="3" t="inlineStr">
         <is>
-          <t>ايهم كريم على</t>
+          <t>شهد حاتم حسن حسن علام</t>
         </is>
       </c>
       <c r="C94" s="3" t="inlineStr">
@@ -2971,7 +3028,7 @@
       </c>
       <c r="B95" s="4" t="inlineStr">
         <is>
-          <t>ثريا محمد عبد النبي ابراهيم حامد</t>
+          <t>سجى محمد ابراهيم حسن يوسف</t>
         </is>
       </c>
       <c r="C95" s="4" t="inlineStr">
@@ -2998,7 +3055,7 @@
       </c>
       <c r="B96" s="3" t="inlineStr">
         <is>
-          <t>Hamza Muhumed Dahir</t>
+          <t xml:space="preserve">رنيم حسام احمد حلمى عبد الحميد </t>
         </is>
       </c>
       <c r="C96" s="3" t="inlineStr">
@@ -3025,7 +3082,7 @@
       </c>
       <c r="B97" s="4" t="inlineStr">
         <is>
-          <t>نوران بنت اشرف بن محمد عثمان</t>
+          <t>سعود خالد سعود الجبور</t>
         </is>
       </c>
       <c r="C97" s="4" t="inlineStr">
@@ -3052,7 +3109,7 @@
       </c>
       <c r="B98" s="3" t="inlineStr">
         <is>
-          <t>الحسن خالد على حزام</t>
+          <t>غفران بنت عبد العزيز بن عبد الرحيم سندى</t>
         </is>
       </c>
       <c r="C98" s="3" t="inlineStr">
@@ -3074,12 +3131,12 @@
     <row r="99">
       <c r="A99" s="4" t="inlineStr">
         <is>
-          <t>211360</t>
+          <t>210768</t>
         </is>
       </c>
       <c r="B99" s="4" t="inlineStr">
         <is>
-          <t>بسنت عاطف حميده محمود</t>
+          <t>يارا طارق محمد لطفى</t>
         </is>
       </c>
       <c r="C99" s="4" t="inlineStr">
@@ -3106,7 +3163,7 @@
       </c>
       <c r="B100" s="3" t="inlineStr">
         <is>
-          <t>يارا طارق محمد لطفى</t>
+          <t>على احمد نجاح الشاعر</t>
         </is>
       </c>
       <c r="C100" s="3" t="inlineStr">
@@ -3133,7 +3190,7 @@
       </c>
       <c r="B101" s="4" t="inlineStr">
         <is>
-          <t>على احمد نجاح الشاعر</t>
+          <t>عمر طارق عباس سيد</t>
         </is>
       </c>
       <c r="C101" s="4" t="inlineStr">
@@ -3160,7 +3217,7 @@
       </c>
       <c r="B102" s="3" t="inlineStr">
         <is>
-          <t>عمر طارق عباس سيد</t>
+          <t>سما اسامه محمد ذكى</t>
         </is>
       </c>
       <c r="C102" s="3" t="inlineStr">
@@ -3187,7 +3244,7 @@
       </c>
       <c r="B103" s="4" t="inlineStr">
         <is>
-          <t>سما اسامه محمد ذكى</t>
+          <t>نوران مؤمن امين اسماعيل عليوة</t>
         </is>
       </c>
       <c r="C103" s="4" t="inlineStr">
@@ -3214,7 +3271,7 @@
       </c>
       <c r="B104" s="3" t="inlineStr">
         <is>
-          <t>نوران مؤمن امين اسماعيل عليوة</t>
+          <t>كريم حسين عوض الله عوض الله الوحش</t>
         </is>
       </c>
       <c r="C104" s="3" t="inlineStr">
@@ -3241,7 +3298,7 @@
       </c>
       <c r="B105" s="4" t="inlineStr">
         <is>
-          <t>كريم حسين عوض الله عوض الله الوحش</t>
+          <t>زينب فراج محمد عبد الرءوف</t>
         </is>
       </c>
       <c r="C105" s="4" t="inlineStr">
@@ -3268,7 +3325,7 @@
       </c>
       <c r="B106" s="3" t="inlineStr">
         <is>
-          <t>زينب فراج محمد عبد الرءوف</t>
+          <t>لوجين ايمن حافظ احمد شلبى</t>
         </is>
       </c>
       <c r="C106" s="3" t="inlineStr">
@@ -3295,7 +3352,7 @@
       </c>
       <c r="B107" s="4" t="inlineStr">
         <is>
-          <t>لوجين ايمن حافظ احمد شلبى</t>
+          <t>مريم ايهاب فكرى ابراهيم بيومى</t>
         </is>
       </c>
       <c r="C107" s="4" t="inlineStr">
@@ -3322,7 +3379,7 @@
       </c>
       <c r="B108" s="3" t="inlineStr">
         <is>
-          <t>مريم ايهاب فكرى ابراهيم بيومى</t>
+          <t>محمد احمد سيكوتورى محمود احمد</t>
         </is>
       </c>
       <c r="C108" s="3" t="inlineStr">
@@ -3349,7 +3406,7 @@
       </c>
       <c r="B109" s="4" t="inlineStr">
         <is>
-          <t>محمد احمد سيكوتورى محمود احمد</t>
+          <t>سيف الدين محمد اسماعيل زكى</t>
         </is>
       </c>
       <c r="C109" s="4" t="inlineStr">
@@ -3376,7 +3433,7 @@
       </c>
       <c r="B110" s="3" t="inlineStr">
         <is>
-          <t>سيف الدين محمد اسماعيل زكى</t>
+          <t>سلمى شريف جابر عبد الرحمن احمد</t>
         </is>
       </c>
       <c r="C110" s="3" t="inlineStr">
@@ -3403,7 +3460,7 @@
       </c>
       <c r="B111" s="4" t="inlineStr">
         <is>
-          <t>سلمى شريف جابر عبد الرحمن احمد</t>
+          <t>بيتر ايمن ماهر عياد عطا الله</t>
         </is>
       </c>
       <c r="C111" s="4" t="inlineStr">
@@ -3430,7 +3487,7 @@
       </c>
       <c r="B112" s="3" t="inlineStr">
         <is>
-          <t>بيتر ايمن ماهر عياد عطا الله</t>
+          <t>بافلى نبيل فاروق نجيب عوض</t>
         </is>
       </c>
       <c r="C112" s="3" t="inlineStr">
@@ -3457,7 +3514,7 @@
       </c>
       <c r="B113" s="4" t="inlineStr">
         <is>
-          <t>بافلى نبيل فاروق نجيب عوض</t>
+          <t>شمس الدين حجازى عبد الحميد سعد الجزار</t>
         </is>
       </c>
       <c r="C113" s="4" t="inlineStr">
@@ -3484,7 +3541,7 @@
       </c>
       <c r="B114" s="3" t="inlineStr">
         <is>
-          <t>شمس الدين حجازى عبد الحميد سعد الجزار</t>
+          <t>ملك هيثم احمد ابو الفضل</t>
         </is>
       </c>
       <c r="C114" s="3" t="inlineStr">
@@ -3511,7 +3568,7 @@
       </c>
       <c r="B115" s="4" t="inlineStr">
         <is>
-          <t>ملك هيثم احمد ابو الفضل</t>
+          <t>نور ابراهيم احمد ابراهيم فهمى المنير</t>
         </is>
       </c>
       <c r="C115" s="4" t="inlineStr">
@@ -3538,7 +3595,7 @@
       </c>
       <c r="B116" s="3" t="inlineStr">
         <is>
-          <t>نور ابراهيم احمد ابراهيم فهمى المنير</t>
+          <t>مريم تامر يوسف محمد ابراهيم</t>
         </is>
       </c>
       <c r="C116" s="3" t="inlineStr">
@@ -3565,7 +3622,7 @@
       </c>
       <c r="B117" s="4" t="inlineStr">
         <is>
-          <t>مريم تامر يوسف محمد ابراهيم</t>
+          <t xml:space="preserve">مريم معتز محمود محمد ابراهيم </t>
         </is>
       </c>
       <c r="C117" s="4" t="inlineStr">
@@ -3592,7 +3649,7 @@
       </c>
       <c r="B118" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">مريم معتز محمود محمد ابراهيم </t>
+          <t>احمد محمد عبد العزيز التحيوى</t>
         </is>
       </c>
       <c r="C118" s="3" t="inlineStr">
@@ -3619,7 +3676,7 @@
       </c>
       <c r="B119" s="4" t="inlineStr">
         <is>
-          <t>احمد محمد عبد العزيز التحيوى</t>
+          <t>محمد محمد عبد السميع محمد جمعه</t>
         </is>
       </c>
       <c r="C119" s="4" t="inlineStr">
@@ -3646,7 +3703,7 @@
       </c>
       <c r="B120" s="3" t="inlineStr">
         <is>
-          <t>محمد محمد عبد السميع محمد جمعه</t>
+          <t>مى حسام رشدى على</t>
         </is>
       </c>
       <c r="C120" s="3" t="inlineStr">
@@ -3673,7 +3730,7 @@
       </c>
       <c r="B121" s="4" t="inlineStr">
         <is>
-          <t>مى حسام رشدى على</t>
+          <t>فرح محمد حسن عبد العزيز</t>
         </is>
       </c>
       <c r="C121" s="4" t="inlineStr">
@@ -3700,7 +3757,7 @@
       </c>
       <c r="B122" s="3" t="inlineStr">
         <is>
-          <t>فرح محمد حسن عبد العزيز</t>
+          <t>عمرو خالد محمد اسماعيل</t>
         </is>
       </c>
       <c r="C122" s="3" t="inlineStr">
@@ -3727,7 +3784,7 @@
       </c>
       <c r="B123" s="4" t="inlineStr">
         <is>
-          <t>عمرو خالد محمد اسماعيل</t>
+          <t>شيرى اغر احمد الجمال</t>
         </is>
       </c>
       <c r="C123" s="4" t="inlineStr">
@@ -3754,7 +3811,7 @@
       </c>
       <c r="B124" s="3" t="inlineStr">
         <is>
-          <t>شيرى اغر احمد الجمال</t>
+          <t>احمد راغب عبد الرحمن راغب ناصف</t>
         </is>
       </c>
       <c r="C124" s="3" t="inlineStr">
@@ -3781,7 +3838,7 @@
       </c>
       <c r="B125" s="4" t="inlineStr">
         <is>
-          <t>احمد راغب عبد الرحمن راغب ناصف</t>
+          <t>عمار محمد حسيب سليمان</t>
         </is>
       </c>
       <c r="C125" s="4" t="inlineStr">
@@ -3808,7 +3865,7 @@
       </c>
       <c r="B126" s="3" t="inlineStr">
         <is>
-          <t>عمار محمد حسيب سليمان</t>
+          <t>حبيبه خالد محمد فتحى عبد النعيم</t>
         </is>
       </c>
       <c r="C126" s="3" t="inlineStr">
@@ -3835,7 +3892,7 @@
       </c>
       <c r="B127" s="4" t="inlineStr">
         <is>
-          <t>حبيبه خالد محمد فتحى عبد النعيم</t>
+          <t>سلمى اشرف امين عبد المجيد</t>
         </is>
       </c>
       <c r="C127" s="4" t="inlineStr">
@@ -3862,7 +3919,7 @@
       </c>
       <c r="B128" s="3" t="inlineStr">
         <is>
-          <t>سلمى اشرف امين عبد المجيد</t>
+          <t>جنه ياسر احمد امين العاصى</t>
         </is>
       </c>
       <c r="C128" s="3" t="inlineStr">
@@ -3889,7 +3946,7 @@
       </c>
       <c r="B129" s="4" t="inlineStr">
         <is>
-          <t>جنه ياسر احمد امين العاصى</t>
+          <t>بسنت عاطف حميده محمود</t>
         </is>
       </c>
       <c r="C129" s="4" t="inlineStr">
@@ -3911,12 +3968,12 @@
     <row r="130">
       <c r="A130" s="3" t="inlineStr">
         <is>
-          <t>210554</t>
+          <t>211360</t>
         </is>
       </c>
       <c r="B130" s="3" t="inlineStr">
         <is>
-          <t>فريده احمد محمد فهمى محمد</t>
+          <t>احمد صالح ابراهيم عبد الرحيم خالد</t>
         </is>
       </c>
       <c r="C130" s="3" t="inlineStr">
@@ -3938,12 +3995,12 @@
     <row r="131">
       <c r="A131" s="4" t="inlineStr">
         <is>
-          <t>211408</t>
+          <t>211364</t>
         </is>
       </c>
       <c r="B131" s="4" t="inlineStr">
         <is>
-          <t>احمد صالح ابراهيم عبد الرحيم خالد</t>
+          <t>مريم شادى رزق الباز</t>
         </is>
       </c>
       <c r="C131" s="4" t="inlineStr">
@@ -3965,12 +4022,12 @@
     <row r="132">
       <c r="A132" s="3" t="inlineStr">
         <is>
-          <t>211410</t>
+          <t>211408</t>
         </is>
       </c>
       <c r="B132" s="3" t="inlineStr">
         <is>
-          <t>مريم شادى رزق الباز</t>
+          <t>جولى حسام حلمى حبيب</t>
         </is>
       </c>
       <c r="C132" s="3" t="inlineStr">
@@ -3992,12 +4049,12 @@
     <row r="133">
       <c r="A133" s="4" t="inlineStr">
         <is>
-          <t>211411</t>
+          <t>211410</t>
         </is>
       </c>
       <c r="B133" s="4" t="inlineStr">
         <is>
-          <t>جولى حسام حلمى حبيب</t>
+          <t>جون مجدى ميخائيل سدراك</t>
         </is>
       </c>
       <c r="C133" s="4" t="inlineStr">
@@ -4019,12 +4076,12 @@
     <row r="134">
       <c r="A134" s="3" t="inlineStr">
         <is>
-          <t>211412</t>
+          <t>211411</t>
         </is>
       </c>
       <c r="B134" s="3" t="inlineStr">
         <is>
-          <t>جون مجدى ميخائيل سدراك</t>
+          <t>روان عبد الله طه هيكل</t>
         </is>
       </c>
       <c r="C134" s="3" t="inlineStr">
@@ -4046,12 +4103,12 @@
     <row r="135">
       <c r="A135" s="4" t="inlineStr">
         <is>
-          <t>211416</t>
+          <t>211412</t>
         </is>
       </c>
       <c r="B135" s="4" t="inlineStr">
         <is>
-          <t>روان عبد الله طه هيكل</t>
+          <t>نوران اشرف سيد على عثمان</t>
         </is>
       </c>
       <c r="C135" s="4" t="inlineStr">
@@ -4073,12 +4130,12 @@
     <row r="136">
       <c r="A136" s="3" t="inlineStr">
         <is>
-          <t>211418</t>
+          <t>211416</t>
         </is>
       </c>
       <c r="B136" s="3" t="inlineStr">
         <is>
-          <t>نوران اشرف سيد على عثمان</t>
+          <t>لبنى محمود محمود امين</t>
         </is>
       </c>
       <c r="C136" s="3" t="inlineStr">
@@ -4100,12 +4157,12 @@
     <row r="137">
       <c r="A137" s="4" t="inlineStr">
         <is>
-          <t>211420</t>
+          <t>211418</t>
         </is>
       </c>
       <c r="B137" s="4" t="inlineStr">
         <is>
-          <t>لبنى محمود محمود امين</t>
+          <t>احمد علاء عبد الله زكى عبده</t>
         </is>
       </c>
       <c r="C137" s="4" t="inlineStr">
@@ -4127,12 +4184,12 @@
     <row r="138">
       <c r="A138" s="3" t="inlineStr">
         <is>
-          <t>211422</t>
+          <t>211420</t>
         </is>
       </c>
       <c r="B138" s="3" t="inlineStr">
         <is>
-          <t>احمد علاء عبد الله زكى عبده</t>
+          <t>مريم هشام احمد الخولى</t>
         </is>
       </c>
       <c r="C138" s="3" t="inlineStr">
@@ -4154,12 +4211,12 @@
     <row r="139">
       <c r="A139" s="4" t="inlineStr">
         <is>
-          <t>211424</t>
+          <t>211422</t>
         </is>
       </c>
       <c r="B139" s="4" t="inlineStr">
         <is>
-          <t>مريم هشام احمد الخولى</t>
+          <t>احمد حسام ابراهيم عبد العزيز ابراهيم</t>
         </is>
       </c>
       <c r="C139" s="4" t="inlineStr">
@@ -4181,12 +4238,12 @@
     <row r="140">
       <c r="A140" s="3" t="inlineStr">
         <is>
-          <t>211427</t>
+          <t>211424</t>
         </is>
       </c>
       <c r="B140" s="3" t="inlineStr">
         <is>
-          <t>احمد حسام ابراهيم عبد العزيز ابراهيم</t>
+          <t>دعاء اشرف حامد صديق توفيق</t>
         </is>
       </c>
       <c r="C140" s="3" t="inlineStr">
@@ -4208,12 +4265,12 @@
     <row r="141">
       <c r="A141" s="4" t="inlineStr">
         <is>
-          <t>211428</t>
+          <t>211427</t>
         </is>
       </c>
       <c r="B141" s="4" t="inlineStr">
         <is>
-          <t>دعاء اشرف حامد صديق توفيق</t>
+          <t>حسام خالد سعد محمد خليل</t>
         </is>
       </c>
       <c r="C141" s="4" t="inlineStr">
@@ -4235,12 +4292,12 @@
     <row r="142">
       <c r="A142" s="3" t="inlineStr">
         <is>
-          <t>211429</t>
+          <t>211428</t>
         </is>
       </c>
       <c r="B142" s="3" t="inlineStr">
         <is>
-          <t>يوستينا ماجد نصر محروس حنا</t>
+          <t>عمرو محمود لبيب عبد الستار علم الدين</t>
         </is>
       </c>
       <c r="C142" s="3" t="inlineStr">
@@ -4267,7 +4324,7 @@
       </c>
       <c r="B143" s="4" t="inlineStr">
         <is>
-          <t>حسام خالد سعد محمد خليل</t>
+          <t>نور وليد خميس عبد المحسن</t>
         </is>
       </c>
       <c r="C143" s="4" t="inlineStr">
@@ -4294,7 +4351,7 @@
       </c>
       <c r="B144" s="3" t="inlineStr">
         <is>
-          <t>عمرو محمود لبيب عبد الستار علم الدين</t>
+          <t>عبد الله احمد طلعت الشوره</t>
         </is>
       </c>
       <c r="C144" s="3" t="inlineStr">
@@ -4321,7 +4378,7 @@
       </c>
       <c r="B145" s="4" t="inlineStr">
         <is>
-          <t>نور وليد خميس عبد المحسن</t>
+          <t>نورا هانى محمد نبيل الحناوى</t>
         </is>
       </c>
       <c r="C145" s="4" t="inlineStr">
@@ -4348,7 +4405,7 @@
       </c>
       <c r="B146" s="3" t="inlineStr">
         <is>
-          <t>عبد الله احمد طلعت الشوره</t>
+          <t>ياسمين محمد احمد عوض</t>
         </is>
       </c>
       <c r="C146" s="3" t="inlineStr">
@@ -4375,7 +4432,7 @@
       </c>
       <c r="B147" s="4" t="inlineStr">
         <is>
-          <t>نورا هانى محمد نبيل الحناوى</t>
+          <t>احمد عمرو احمد حجازى مرسى</t>
         </is>
       </c>
       <c r="C147" s="4" t="inlineStr">
@@ -4402,7 +4459,7 @@
       </c>
       <c r="B148" s="3" t="inlineStr">
         <is>
-          <t>ياسمين محمد احمد عوض</t>
+          <t>عبد الرحمن سامح عبد العزيز منصور</t>
         </is>
       </c>
       <c r="C148" s="3" t="inlineStr">
@@ -4429,7 +4486,7 @@
       </c>
       <c r="B149" s="4" t="inlineStr">
         <is>
-          <t>احمد عمرو احمد حجازى مرسى</t>
+          <t>دينا عادل طلخان رزق</t>
         </is>
       </c>
       <c r="C149" s="4" t="inlineStr">
@@ -4456,7 +4513,7 @@
       </c>
       <c r="B150" s="3" t="inlineStr">
         <is>
-          <t>عبد الرحمن سامح عبد العزيز منصور</t>
+          <t>غاده عصام عمروسى ابراهيم محسن</t>
         </is>
       </c>
       <c r="C150" s="3" t="inlineStr">
@@ -4483,7 +4540,7 @@
       </c>
       <c r="B151" s="4" t="inlineStr">
         <is>
-          <t>دينا عادل طلخان رزق</t>
+          <t>بسمله ياسر محمد محمد عبد السلام</t>
         </is>
       </c>
       <c r="C151" s="4" t="inlineStr">
@@ -4510,7 +4567,7 @@
       </c>
       <c r="B152" s="3" t="inlineStr">
         <is>
-          <t>غاده عصام عمروسى ابراهيم محسن</t>
+          <t>مريم محمد نور الدين محمد حسن عبد الرحيم</t>
         </is>
       </c>
       <c r="C152" s="3" t="inlineStr">
@@ -4537,7 +4594,7 @@
       </c>
       <c r="B153" s="4" t="inlineStr">
         <is>
-          <t>بسمله ياسر محمد محمد عبد السلام</t>
+          <t>ساره عبد الله محمد كمال عبد العزيز</t>
         </is>
       </c>
       <c r="C153" s="4" t="inlineStr">
@@ -4564,7 +4621,7 @@
       </c>
       <c r="B154" s="3" t="inlineStr">
         <is>
-          <t>مريم محمد نور الدين محمد حسن عبد الرحيم</t>
+          <t xml:space="preserve">حبيبه محمود على محمد </t>
         </is>
       </c>
       <c r="C154" s="3" t="inlineStr">
@@ -4591,7 +4648,7 @@
       </c>
       <c r="B155" s="4" t="inlineStr">
         <is>
-          <t>ساره عبد الله محمد كمال عبد العزيز</t>
+          <t>مريم احمد عادل عبد المقصود الخيارى</t>
         </is>
       </c>
       <c r="C155" s="4" t="inlineStr">
@@ -4618,7 +4675,7 @@
       </c>
       <c r="B156" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">حبيبه محمود على محمد </t>
+          <t>فريده احمد محمد فهمى محمد</t>
         </is>
       </c>
       <c r="C156" s="3" t="inlineStr">
@@ -4645,7 +4702,7 @@
       </c>
       <c r="B157" s="4" t="inlineStr">
         <is>
-          <t>مريم احمد عادل عبد المقصود الخيارى</t>
+          <t>يوستينا ماجد نصر محروس حنا</t>
         </is>
       </c>
       <c r="C157" s="4" t="inlineStr">
@@ -4667,12 +4724,12 @@
     <row r="158">
       <c r="A158" s="3" t="inlineStr">
         <is>
-          <t>210758</t>
+          <t>210554</t>
         </is>
       </c>
       <c r="B158" s="3" t="inlineStr">
         <is>
-          <t>عادل حسن مجدى السيد شرشر</t>
+          <t>علا محمد عثمان ابراهيم</t>
         </is>
       </c>
       <c r="C158" s="3" t="inlineStr">
@@ -4694,12 +4751,12 @@
     <row r="159">
       <c r="A159" s="4" t="inlineStr">
         <is>
-          <t>211413</t>
+          <t>211429</t>
         </is>
       </c>
       <c r="B159" s="4" t="inlineStr">
         <is>
-          <t>منه الله شريف محمد صالح جاد عبد الله</t>
+          <t>سلمى محسن عاشور حسن</t>
         </is>
       </c>
       <c r="C159" s="4" t="inlineStr">
@@ -4721,12 +4778,12 @@
     <row r="160">
       <c r="A160" s="3" t="inlineStr">
         <is>
-          <t>211447</t>
+          <t>211433</t>
         </is>
       </c>
       <c r="B160" s="3" t="inlineStr">
         <is>
-          <t>علا محمد عثمان ابراهيم</t>
+          <t>يوسف احمد حلمى جلال حلمى سلام</t>
         </is>
       </c>
       <c r="C160" s="3" t="inlineStr">
@@ -4748,12 +4805,12 @@
     <row r="161">
       <c r="A161" s="4" t="inlineStr">
         <is>
-          <t>211452</t>
+          <t>211447</t>
         </is>
       </c>
       <c r="B161" s="4" t="inlineStr">
         <is>
-          <t>سلمى محسن عاشور حسن</t>
+          <t>روان عاطف عبد الحميد احمد</t>
         </is>
       </c>
       <c r="C161" s="4" t="inlineStr">
@@ -4775,12 +4832,12 @@
     <row r="162">
       <c r="A162" s="3" t="inlineStr">
         <is>
-          <t>211454</t>
+          <t>211452</t>
         </is>
       </c>
       <c r="B162" s="3" t="inlineStr">
         <is>
-          <t>كمال ماهر كمال ابراهيم</t>
+          <t>عمرو رجائى محمد فريد عبد المجيد فراج</t>
         </is>
       </c>
       <c r="C162" s="3" t="inlineStr">
@@ -4807,7 +4864,7 @@
       </c>
       <c r="B163" s="4" t="inlineStr">
         <is>
-          <t>يوسف احمد حلمى جلال حلمى سلام</t>
+          <t>اسماء مرتضى فتحى صادق</t>
         </is>
       </c>
       <c r="C163" s="4" t="inlineStr">
@@ -4834,7 +4891,7 @@
       </c>
       <c r="B164" s="3" t="inlineStr">
         <is>
-          <t>روان عاطف عبد الحميد احمد</t>
+          <t>حنين محمد رفاعى عبد التواب</t>
         </is>
       </c>
       <c r="C164" s="3" t="inlineStr">
@@ -4861,7 +4918,7 @@
       </c>
       <c r="B165" s="4" t="inlineStr">
         <is>
-          <t>عمرو رجائى محمد فريد عبد المجيد فراج</t>
+          <t>محمد هانى عثمان السيد فضل</t>
         </is>
       </c>
       <c r="C165" s="4" t="inlineStr">
@@ -4888,7 +4945,7 @@
       </c>
       <c r="B166" s="3" t="inlineStr">
         <is>
-          <t>اسماء مرتضى فتحى صادق</t>
+          <t>امير شريف عفت حلمى جرجس</t>
         </is>
       </c>
       <c r="C166" s="3" t="inlineStr">
@@ -4915,7 +4972,7 @@
       </c>
       <c r="B167" s="4" t="inlineStr">
         <is>
-          <t>حنين محمد رفاعى عبد التواب</t>
+          <t>زياد عصام فريد ذكى جاد الله</t>
         </is>
       </c>
       <c r="C167" s="4" t="inlineStr">
@@ -4942,7 +4999,7 @@
       </c>
       <c r="B168" s="3" t="inlineStr">
         <is>
-          <t>محمد هانى عثمان السيد فضل</t>
+          <t>محمد ايمن رمضان محمد حسن</t>
         </is>
       </c>
       <c r="C168" s="3" t="inlineStr">
@@ -4969,7 +5026,7 @@
       </c>
       <c r="B169" s="4" t="inlineStr">
         <is>
-          <t>امير شريف عفت حلمى جرجس</t>
+          <t>سهيله ايمن احمد يوسف احمد</t>
         </is>
       </c>
       <c r="C169" s="4" t="inlineStr">
@@ -4996,7 +5053,7 @@
       </c>
       <c r="B170" s="3" t="inlineStr">
         <is>
-          <t>زياد عصام فريد ذكى جاد الله</t>
+          <t>نور الدين محمد سامى محمد عز الدين</t>
         </is>
       </c>
       <c r="C170" s="3" t="inlineStr">
@@ -5023,7 +5080,7 @@
       </c>
       <c r="B171" s="4" t="inlineStr">
         <is>
-          <t>محمد ايمن رمضان محمد حسن</t>
+          <t>نانسى محمد رجب احمد العدوى</t>
         </is>
       </c>
       <c r="C171" s="4" t="inlineStr">
@@ -5050,7 +5107,7 @@
       </c>
       <c r="B172" s="3" t="inlineStr">
         <is>
-          <t>سهيله ايمن احمد يوسف احمد</t>
+          <t>مارييت اميل منير راغب</t>
         </is>
       </c>
       <c r="C172" s="3" t="inlineStr">
@@ -5077,7 +5134,7 @@
       </c>
       <c r="B173" s="4" t="inlineStr">
         <is>
-          <t>نور الدين محمد سامى محمد عز الدين</t>
+          <t>مروان وائل فاروق رضوان</t>
         </is>
       </c>
       <c r="C173" s="4" t="inlineStr">
@@ -5104,7 +5161,7 @@
       </c>
       <c r="B174" s="3" t="inlineStr">
         <is>
-          <t>نانسى محمد رجب احمد العدوى</t>
+          <t>جوردينا عادل عاطف يوسف</t>
         </is>
       </c>
       <c r="C174" s="3" t="inlineStr">
@@ -5131,7 +5188,7 @@
       </c>
       <c r="B175" s="4" t="inlineStr">
         <is>
-          <t>مارييت اميل منير راغب</t>
+          <t>مؤمن الحسينى على الحسينى محمود</t>
         </is>
       </c>
       <c r="C175" s="4" t="inlineStr">
@@ -5158,7 +5215,7 @@
       </c>
       <c r="B176" s="3" t="inlineStr">
         <is>
-          <t>مروان وائل فاروق رضوان</t>
+          <t>نانسى ماهر عبد الرؤف الجمال</t>
         </is>
       </c>
       <c r="C176" s="3" t="inlineStr">
@@ -5185,7 +5242,7 @@
       </c>
       <c r="B177" s="4" t="inlineStr">
         <is>
-          <t>جوردينا عادل عاطف يوسف</t>
+          <t>حنين ياسر ابراهيم مامون</t>
         </is>
       </c>
       <c r="C177" s="4" t="inlineStr">
@@ -5212,7 +5269,7 @@
       </c>
       <c r="B178" s="3" t="inlineStr">
         <is>
-          <t>مؤمن الحسينى على الحسينى محمود</t>
+          <t xml:space="preserve">فرح وليد عمرى محمود احمد حسن </t>
         </is>
       </c>
       <c r="C178" s="3" t="inlineStr">
@@ -5239,7 +5296,7 @@
       </c>
       <c r="B179" s="4" t="inlineStr">
         <is>
-          <t>نانسى ماهر عبد الرؤف الجمال</t>
+          <t>كريم وليد احمد فتحى ابراهيم</t>
         </is>
       </c>
       <c r="C179" s="4" t="inlineStr">
@@ -5266,7 +5323,7 @@
       </c>
       <c r="B180" s="3" t="inlineStr">
         <is>
-          <t>حنين ياسر ابراهيم مامون</t>
+          <t>احمد عمرو محمد محمود شافعى</t>
         </is>
       </c>
       <c r="C180" s="3" t="inlineStr">
@@ -5293,7 +5350,7 @@
       </c>
       <c r="B181" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">فرح وليد عمرى محمود احمد حسن </t>
+          <t>مريم طارق محمد محمد ريحان</t>
         </is>
       </c>
       <c r="C181" s="4" t="inlineStr">
@@ -5320,7 +5377,7 @@
       </c>
       <c r="B182" s="3" t="inlineStr">
         <is>
-          <t>كريم وليد احمد فتحى ابراهيم</t>
+          <t>ليلى الحسين محمد مصطفى الدكرونى</t>
         </is>
       </c>
       <c r="C182" s="3" t="inlineStr">
@@ -5347,7 +5404,7 @@
       </c>
       <c r="B183" s="4" t="inlineStr">
         <is>
-          <t>احمد عمرو محمد محمود شافعى</t>
+          <t>عمر احمد عبد الحكيم محمد زيان</t>
         </is>
       </c>
       <c r="C183" s="4" t="inlineStr">
@@ -5374,7 +5431,7 @@
       </c>
       <c r="B184" s="3" t="inlineStr">
         <is>
-          <t>مريم طارق محمد محمد ريحان</t>
+          <t>عادل حسن مجدى السيد شرشر</t>
         </is>
       </c>
       <c r="C184" s="3" t="inlineStr">
@@ -5401,7 +5458,7 @@
       </c>
       <c r="B185" s="4" t="inlineStr">
         <is>
-          <t>ليلى الحسين محمد مصطفى الدكرونى</t>
+          <t>منه الله شريف محمد صالح جاد عبد الله</t>
         </is>
       </c>
       <c r="C185" s="4" t="inlineStr">
@@ -5428,7 +5485,7 @@
       </c>
       <c r="B186" s="3" t="inlineStr">
         <is>
-          <t>عمر احمد عبد الحكيم محمد زيان</t>
+          <t>كمال ماهر كمال ابراهيم</t>
         </is>
       </c>
       <c r="C186" s="3" t="inlineStr">
@@ -5450,12 +5507,12 @@
     <row r="187">
       <c r="A187" s="4" t="inlineStr">
         <is>
-          <t>200959</t>
+          <t>210758</t>
         </is>
       </c>
       <c r="B187" s="4" t="inlineStr">
         <is>
-          <t>سلمى ايهاب على كيلانى</t>
+          <t>هايدى هانى صبحى صديق</t>
         </is>
       </c>
       <c r="C187" s="4" t="inlineStr">
@@ -5477,12 +5534,12 @@
     <row r="188">
       <c r="A188" s="3" t="inlineStr">
         <is>
-          <t>210294</t>
+          <t>211413</t>
         </is>
       </c>
       <c r="B188" s="3" t="inlineStr">
         <is>
-          <t>شهد احمد مصطفى عزالدين البخشونجى</t>
+          <t>جنى احمد ماهر عبد الوهاب على ابراهيم</t>
         </is>
       </c>
       <c r="C188" s="3" t="inlineStr">
@@ -5504,12 +5561,12 @@
     <row r="189">
       <c r="A189" s="4" t="inlineStr">
         <is>
-          <t>211476</t>
+          <t>211454</t>
         </is>
       </c>
       <c r="B189" s="4" t="inlineStr">
         <is>
-          <t>هايدى هانى صبحى صديق</t>
+          <t>نماء احمد كمال قطب على</t>
         </is>
       </c>
       <c r="C189" s="4" t="inlineStr">
@@ -5531,12 +5588,12 @@
     <row r="190">
       <c r="A190" s="3" t="inlineStr">
         <is>
-          <t>211497</t>
+          <t>211455</t>
         </is>
       </c>
       <c r="B190" s="3" t="inlineStr">
         <is>
-          <t>جنى احمد ماهر عبد الوهاب على ابراهيم</t>
+          <t>هنا محمد محمد توفيق</t>
         </is>
       </c>
       <c r="C190" s="3" t="inlineStr">
@@ -5558,12 +5615,12 @@
     <row r="191">
       <c r="A191" s="4" t="inlineStr">
         <is>
-          <t>211500</t>
+          <t>211476</t>
         </is>
       </c>
       <c r="B191" s="4" t="inlineStr">
         <is>
-          <t>نماء احمد كمال قطب على</t>
+          <t>جنى طارق محمود عبد الرحيم محمد الحبشى</t>
         </is>
       </c>
       <c r="C191" s="4" t="inlineStr">
@@ -5585,12 +5642,12 @@
     <row r="192">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>211501</t>
+          <t>211497</t>
         </is>
       </c>
       <c r="B192" s="3" t="inlineStr">
         <is>
-          <t>هنا محمد محمد توفيق</t>
+          <t>احمد محمد ابو الوفا عبد الغفار ابو الوفا</t>
         </is>
       </c>
       <c r="C192" s="3" t="inlineStr">
@@ -5612,12 +5669,12 @@
     <row r="193">
       <c r="A193" s="4" t="inlineStr">
         <is>
-          <t>211502</t>
+          <t>211500</t>
         </is>
       </c>
       <c r="B193" s="4" t="inlineStr">
         <is>
-          <t>جنى طارق محمود عبد الرحيم محمد الحبشى</t>
+          <t>روان سامى جمال خضر</t>
         </is>
       </c>
       <c r="C193" s="4" t="inlineStr">
@@ -5639,12 +5696,12 @@
     <row r="194">
       <c r="A194" s="3" t="inlineStr">
         <is>
-          <t>211504</t>
+          <t>211501</t>
         </is>
       </c>
       <c r="B194" s="3" t="inlineStr">
         <is>
-          <t>احمد محمد ابو الوفا عبد الغفار ابو الوفا</t>
+          <t>روضه محمد عبد الواحد السعداوى</t>
         </is>
       </c>
       <c r="C194" s="3" t="inlineStr">
@@ -5666,12 +5723,12 @@
     <row r="195">
       <c r="A195" s="4" t="inlineStr">
         <is>
-          <t>211506</t>
+          <t>211502</t>
         </is>
       </c>
       <c r="B195" s="4" t="inlineStr">
         <is>
-          <t>روان سامى جمال خضر</t>
+          <t>نور احمد اسماعيل ابراهيم</t>
         </is>
       </c>
       <c r="C195" s="4" t="inlineStr">
@@ -5693,12 +5750,12 @@
     <row r="196">
       <c r="A196" s="3" t="inlineStr">
         <is>
-          <t>211507</t>
+          <t>211504</t>
         </is>
       </c>
       <c r="B196" s="3" t="inlineStr">
         <is>
-          <t>روضه محمد عبد الواحد السعداوى</t>
+          <t>سما حاتم عبد المجيد السيد مطر</t>
         </is>
       </c>
       <c r="C196" s="3" t="inlineStr">
@@ -5720,12 +5777,12 @@
     <row r="197">
       <c r="A197" s="4" t="inlineStr">
         <is>
-          <t>211508</t>
+          <t>211506</t>
         </is>
       </c>
       <c r="B197" s="4" t="inlineStr">
         <is>
-          <t>نور احمد اسماعيل ابراهيم</t>
+          <t>عبد الرحمن معتز عبد المجيد محمود عبد المجيد</t>
         </is>
       </c>
       <c r="C197" s="4" t="inlineStr">
@@ -5747,12 +5804,12 @@
     <row r="198">
       <c r="A198" s="3" t="inlineStr">
         <is>
-          <t>211510</t>
+          <t>211507</t>
         </is>
       </c>
       <c r="B198" s="3" t="inlineStr">
         <is>
-          <t>سما حاتم عبد المجيد السيد مطر</t>
+          <t>رامى خالد سعد الدين محمد رجب</t>
         </is>
       </c>
       <c r="C198" s="3" t="inlineStr">
@@ -5774,12 +5831,12 @@
     <row r="199">
       <c r="A199" s="4" t="inlineStr">
         <is>
-          <t>211512</t>
+          <t>211508</t>
         </is>
       </c>
       <c r="B199" s="4" t="inlineStr">
         <is>
-          <t>عبد الرحمن معتز عبد المجيد محمود عبد المجيد</t>
+          <t>مارك فادى اديب عبد الملك</t>
         </is>
       </c>
       <c r="C199" s="4" t="inlineStr">
@@ -5801,12 +5858,12 @@
     <row r="200">
       <c r="A200" s="3" t="inlineStr">
         <is>
-          <t>211514</t>
+          <t>211510</t>
         </is>
       </c>
       <c r="B200" s="3" t="inlineStr">
         <is>
-          <t>رامى خالد سعد الدين محمد رجب</t>
+          <t>شهد هشام محمود حسن الوكيل</t>
         </is>
       </c>
       <c r="C200" s="3" t="inlineStr">
@@ -5828,12 +5885,12 @@
     <row r="201">
       <c r="A201" s="4" t="inlineStr">
         <is>
-          <t>211515</t>
+          <t>211512</t>
         </is>
       </c>
       <c r="B201" s="4" t="inlineStr">
         <is>
-          <t>مارك فادى اديب عبد الملك</t>
+          <t>يوسف عادل اسماعيل يوسف</t>
         </is>
       </c>
       <c r="C201" s="4" t="inlineStr">
@@ -5855,12 +5912,12 @@
     <row r="202">
       <c r="A202" s="3" t="inlineStr">
         <is>
-          <t>211516</t>
+          <t>211514</t>
         </is>
       </c>
       <c r="B202" s="3" t="inlineStr">
         <is>
-          <t>شهد هشام محمود حسن الوكيل</t>
+          <t>محمد احمد عبد الله محمد محمد الازرق</t>
         </is>
       </c>
       <c r="C202" s="3" t="inlineStr">
@@ -5882,12 +5939,12 @@
     <row r="203">
       <c r="A203" s="4" t="inlineStr">
         <is>
-          <t>211517</t>
+          <t>211515</t>
         </is>
       </c>
       <c r="B203" s="4" t="inlineStr">
         <is>
-          <t>يوسف عادل اسماعيل يوسف</t>
+          <t>رفيق هانى رفيق حليم واكيم</t>
         </is>
       </c>
       <c r="C203" s="4" t="inlineStr">
@@ -5909,12 +5966,12 @@
     <row r="204">
       <c r="A204" s="3" t="inlineStr">
         <is>
-          <t>211519</t>
+          <t>211516</t>
         </is>
       </c>
       <c r="B204" s="3" t="inlineStr">
         <is>
-          <t>محمد احمد عبد الله محمد محمد الازرق</t>
+          <t>جاسمن محمد مجدى محمد زكى</t>
         </is>
       </c>
       <c r="C204" s="3" t="inlineStr">
@@ -5936,12 +5993,12 @@
     <row r="205">
       <c r="A205" s="4" t="inlineStr">
         <is>
-          <t>211520</t>
+          <t>211517</t>
         </is>
       </c>
       <c r="B205" s="4" t="inlineStr">
         <is>
-          <t>رفيق هانى رفيق حليم واكيم</t>
+          <t>مريم محمد على عبد الرحمن</t>
         </is>
       </c>
       <c r="C205" s="4" t="inlineStr">
@@ -5963,12 +6020,12 @@
     <row r="206">
       <c r="A206" s="3" t="inlineStr">
         <is>
-          <t>211521</t>
+          <t>211519</t>
         </is>
       </c>
       <c r="B206" s="3" t="inlineStr">
         <is>
-          <t>جاسمن محمد مجدى محمد زكى</t>
+          <t>داليا محمد شرف الدين محمد</t>
         </is>
       </c>
       <c r="C206" s="3" t="inlineStr">
@@ -5990,12 +6047,12 @@
     <row r="207">
       <c r="A207" s="4" t="inlineStr">
         <is>
-          <t>211522</t>
+          <t>211520</t>
         </is>
       </c>
       <c r="B207" s="4" t="inlineStr">
         <is>
-          <t>مريم محمد على عبد الرحمن</t>
+          <t>محمد معتز محمد فتحى احمد</t>
         </is>
       </c>
       <c r="C207" s="4" t="inlineStr">
@@ -6017,12 +6074,12 @@
     <row r="208">
       <c r="A208" s="3" t="inlineStr">
         <is>
-          <t>211523</t>
+          <t>211521</t>
         </is>
       </c>
       <c r="B208" s="3" t="inlineStr">
         <is>
-          <t>داليا محمد شرف الدين محمد</t>
+          <t>عمر حسن محمد على احمد</t>
         </is>
       </c>
       <c r="C208" s="3" t="inlineStr">
@@ -6044,12 +6101,12 @@
     <row r="209">
       <c r="A209" s="4" t="inlineStr">
         <is>
-          <t>211524</t>
+          <t>211522</t>
         </is>
       </c>
       <c r="B209" s="4" t="inlineStr">
         <is>
-          <t>محمد معتز محمد فتحى احمد</t>
+          <t>عمرو هشام شاكر محمد</t>
         </is>
       </c>
       <c r="C209" s="4" t="inlineStr">
@@ -6071,12 +6128,12 @@
     <row r="210">
       <c r="A210" s="3" t="inlineStr">
         <is>
-          <t>211525</t>
+          <t>211523</t>
         </is>
       </c>
       <c r="B210" s="3" t="inlineStr">
         <is>
-          <t>عمر حسن محمد على احمد</t>
+          <t>لينه حسام عبد العظيم شكرى</t>
         </is>
       </c>
       <c r="C210" s="3" t="inlineStr">
@@ -6098,12 +6155,12 @@
     <row r="211">
       <c r="A211" s="4" t="inlineStr">
         <is>
-          <t>211526</t>
+          <t>211524</t>
         </is>
       </c>
       <c r="B211" s="4" t="inlineStr">
         <is>
-          <t>عمرو هشام شاكر محمد</t>
+          <t>روان ولاء الدين عبد الفتاح عبد الحليم</t>
         </is>
       </c>
       <c r="C211" s="4" t="inlineStr">
@@ -6125,12 +6182,12 @@
     <row r="212">
       <c r="A212" s="3" t="inlineStr">
         <is>
-          <t>211528</t>
+          <t>211525</t>
         </is>
       </c>
       <c r="B212" s="3" t="inlineStr">
         <is>
-          <t>لينه حسام عبد العظيم شكرى</t>
+          <t>ساره محمد ابراهيم محمد سليم</t>
         </is>
       </c>
       <c r="C212" s="3" t="inlineStr">
@@ -6152,12 +6209,12 @@
     <row r="213">
       <c r="A213" s="4" t="inlineStr">
         <is>
-          <t>211530</t>
+          <t>211526</t>
         </is>
       </c>
       <c r="B213" s="4" t="inlineStr">
         <is>
-          <t>روان ولاء الدين عبد الفتاح عبد الحليم</t>
+          <t>منه الله حمدى محمد صقر محمد الصاوى الهتير</t>
         </is>
       </c>
       <c r="C213" s="4" t="inlineStr">
@@ -6179,12 +6236,12 @@
     <row r="214">
       <c r="A214" s="3" t="inlineStr">
         <is>
-          <t>211531</t>
+          <t>211528</t>
         </is>
       </c>
       <c r="B214" s="3" t="inlineStr">
         <is>
-          <t>ساره محمد ابراهيم محمد سليم</t>
+          <t>ميرنا محمد عادل عبد الفتاح</t>
         </is>
       </c>
       <c r="C214" s="3" t="inlineStr">
@@ -6206,12 +6263,12 @@
     <row r="215">
       <c r="A215" s="4" t="inlineStr">
         <is>
-          <t>211532</t>
+          <t>211530</t>
         </is>
       </c>
       <c r="B215" s="4" t="inlineStr">
         <is>
-          <t>محمد عبد الله محمد الجثام</t>
+          <t>احمد رشاد محمود ابراهيم طلبه</t>
         </is>
       </c>
       <c r="C215" s="4" t="inlineStr">
@@ -6233,12 +6290,12 @@
     <row r="216">
       <c r="A216" s="3" t="inlineStr">
         <is>
-          <t>211535</t>
+          <t>211531</t>
         </is>
       </c>
       <c r="B216" s="3" t="inlineStr">
         <is>
-          <t>انطونى رفيق كمال فخرى</t>
+          <t>سلمى ايهاب على كيلانى</t>
         </is>
       </c>
       <c r="C216" s="3" t="inlineStr">
@@ -6265,7 +6322,7 @@
       </c>
       <c r="B217" s="4" t="inlineStr">
         <is>
-          <t>منه الله حمدى محمد صقر محمد الصاوى الهتير</t>
+          <t>شهد احمد مصطفى عزالدين البخشونجى</t>
         </is>
       </c>
       <c r="C217" s="4" t="inlineStr">
@@ -6292,7 +6349,7 @@
       </c>
       <c r="B218" s="3" t="inlineStr">
         <is>
-          <t>ميرنا محمد عادل عبد الفتاح</t>
+          <t>محمد عبد الله محمد الجثام</t>
         </is>
       </c>
       <c r="C218" s="3" t="inlineStr">
@@ -6319,7 +6376,7 @@
       </c>
       <c r="B219" s="4" t="inlineStr">
         <is>
-          <t>احمد رشاد محمود ابراهيم طلبه</t>
+          <t>انطونى رفيق كمال فخرى</t>
         </is>
       </c>
       <c r="C219" s="4" t="inlineStr">
@@ -6341,7 +6398,7 @@
     <row r="220">
       <c r="A220" s="3" t="inlineStr">
         <is>
-          <t>211537</t>
+          <t>200959</t>
         </is>
       </c>
       <c r="B220" s="3" t="inlineStr">
@@ -6368,7 +6425,7 @@
     <row r="221">
       <c r="A221" s="4" t="inlineStr">
         <is>
-          <t>211541</t>
+          <t>210294</t>
         </is>
       </c>
       <c r="B221" s="4" t="inlineStr">
@@ -6395,7 +6452,7 @@
     <row r="222">
       <c r="A222" s="3" t="inlineStr">
         <is>
-          <t>211542</t>
+          <t>211532</t>
         </is>
       </c>
       <c r="B222" s="3" t="inlineStr">
@@ -6422,7 +6479,7 @@
     <row r="223">
       <c r="A223" s="4" t="inlineStr">
         <is>
-          <t>211543</t>
+          <t>211535</t>
         </is>
       </c>
       <c r="B223" s="4" t="inlineStr">
@@ -6449,7 +6506,7 @@
     <row r="224">
       <c r="A224" s="3" t="inlineStr">
         <is>
-          <t>211544</t>
+          <t>211536</t>
         </is>
       </c>
       <c r="B224" s="3" t="inlineStr">
@@ -6476,7 +6533,7 @@
     <row r="225">
       <c r="A225" s="4" t="inlineStr">
         <is>
-          <t>211545</t>
+          <t>211537</t>
         </is>
       </c>
       <c r="B225" s="4" t="inlineStr">
@@ -6503,7 +6560,7 @@
     <row r="226">
       <c r="A226" s="3" t="inlineStr">
         <is>
-          <t>211546</t>
+          <t>211541</t>
         </is>
       </c>
       <c r="B226" s="3" t="inlineStr">
@@ -6530,7 +6587,7 @@
     <row r="227">
       <c r="A227" s="4" t="inlineStr">
         <is>
-          <t>211548</t>
+          <t>211542</t>
         </is>
       </c>
       <c r="B227" s="4" t="inlineStr">
@@ -6557,7 +6614,7 @@
     <row r="228">
       <c r="A228" s="3" t="inlineStr">
         <is>
-          <t>211549</t>
+          <t>211543</t>
         </is>
       </c>
       <c r="B228" s="3" t="inlineStr">
@@ -6584,7 +6641,7 @@
     <row r="229">
       <c r="A229" s="4" t="inlineStr">
         <is>
-          <t>211550</t>
+          <t>211544</t>
         </is>
       </c>
       <c r="B229" s="4" t="inlineStr">
@@ -6611,7 +6668,7 @@
     <row r="230">
       <c r="A230" s="3" t="inlineStr">
         <is>
-          <t>211551</t>
+          <t>211545</t>
         </is>
       </c>
       <c r="B230" s="3" t="inlineStr">
@@ -6638,7 +6695,7 @@
     <row r="231">
       <c r="A231" s="4" t="inlineStr">
         <is>
-          <t>211552</t>
+          <t>211546</t>
         </is>
       </c>
       <c r="B231" s="4" t="inlineStr">
@@ -6665,7 +6722,7 @@
     <row r="232">
       <c r="A232" s="3" t="inlineStr">
         <is>
-          <t>211556</t>
+          <t>211548</t>
         </is>
       </c>
       <c r="B232" s="3" t="inlineStr">
@@ -6692,7 +6749,7 @@
     <row r="233">
       <c r="A233" s="4" t="inlineStr">
         <is>
-          <t>211570</t>
+          <t>211549</t>
         </is>
       </c>
       <c r="B233" s="4" t="inlineStr">
@@ -6719,7 +6776,7 @@
     <row r="234">
       <c r="A234" s="3" t="inlineStr">
         <is>
-          <t>211571</t>
+          <t>211550</t>
         </is>
       </c>
       <c r="B234" s="3" t="inlineStr">
@@ -6746,7 +6803,7 @@
     <row r="235">
       <c r="A235" s="4" t="inlineStr">
         <is>
-          <t>211574</t>
+          <t>211551</t>
         </is>
       </c>
       <c r="B235" s="4" t="inlineStr">
@@ -6773,7 +6830,7 @@
     <row r="236">
       <c r="A236" s="3" t="inlineStr">
         <is>
-          <t>211576</t>
+          <t>211552</t>
         </is>
       </c>
       <c r="B236" s="3" t="inlineStr">
@@ -6800,7 +6857,7 @@
     <row r="237">
       <c r="A237" s="4" t="inlineStr">
         <is>
-          <t>211583</t>
+          <t>211556</t>
         </is>
       </c>
       <c r="B237" s="4" t="inlineStr">
@@ -6827,7 +6884,7 @@
     <row r="238">
       <c r="A238" s="3" t="inlineStr">
         <is>
-          <t>211584</t>
+          <t>211570</t>
         </is>
       </c>
       <c r="B238" s="3" t="inlineStr">
@@ -6854,7 +6911,7 @@
     <row r="239">
       <c r="A239" s="4" t="inlineStr">
         <is>
-          <t>211587</t>
+          <t>211571</t>
         </is>
       </c>
       <c r="B239" s="4" t="inlineStr">
@@ -6881,7 +6938,7 @@
     <row r="240">
       <c r="A240" s="3" t="inlineStr">
         <is>
-          <t>211589</t>
+          <t>211574</t>
         </is>
       </c>
       <c r="B240" s="3" t="inlineStr">
@@ -6908,7 +6965,7 @@
     <row r="241">
       <c r="A241" s="4" t="inlineStr">
         <is>
-          <t>211591</t>
+          <t>211576</t>
         </is>
       </c>
       <c r="B241" s="4" t="inlineStr">
@@ -6935,7 +6992,7 @@
     <row r="242">
       <c r="A242" s="3" t="inlineStr">
         <is>
-          <t>211592</t>
+          <t>211583</t>
         </is>
       </c>
       <c r="B242" s="3" t="inlineStr">
@@ -6962,12 +7019,12 @@
     <row r="243">
       <c r="A243" s="4" t="inlineStr">
         <is>
-          <t>211599</t>
+          <t>211584</t>
         </is>
       </c>
       <c r="B243" s="4" t="inlineStr">
         <is>
-          <t>محمد علاء محمد عبدالدايم</t>
+          <t>احمد عبدالرحيم عمر بن قاضي</t>
         </is>
       </c>
       <c r="C243" s="4" t="inlineStr">
@@ -6989,12 +7046,12 @@
     <row r="244">
       <c r="A244" s="3" t="inlineStr">
         <is>
-          <t>211600</t>
+          <t>211587</t>
         </is>
       </c>
       <c r="B244" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Shoroag Hussein Hassan </t>
+          <t>عبد الله يوسف محمد الدهام</t>
         </is>
       </c>
       <c r="C244" s="3" t="inlineStr">
@@ -7016,12 +7073,12 @@
     <row r="245">
       <c r="A245" s="4" t="inlineStr">
         <is>
-          <t>211601</t>
+          <t>211589</t>
         </is>
       </c>
       <c r="B245" s="4" t="inlineStr">
         <is>
-          <t>على اكرم فتحى شبكى</t>
+          <t>محمد علاء محمد عبدالدايم</t>
         </is>
       </c>
       <c r="C245" s="4" t="inlineStr">
@@ -7043,12 +7100,12 @@
     <row r="246">
       <c r="A246" s="3" t="inlineStr">
         <is>
-          <t>211602</t>
+          <t>211591</t>
         </is>
       </c>
       <c r="B246" s="3" t="inlineStr">
         <is>
-          <t>مريم احمد عبد المنعم عبد السلام عمار</t>
+          <t xml:space="preserve">Shoroag Hussein Hassan </t>
         </is>
       </c>
       <c r="C246" s="3" t="inlineStr">
@@ -7070,12 +7127,12 @@
     <row r="247">
       <c r="A247" s="4" t="inlineStr">
         <is>
-          <t>211605</t>
+          <t>211592</t>
         </is>
       </c>
       <c r="B247" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">جنه وائل كرم محمد فريد </t>
+          <t>على اكرم فتحى شبكى</t>
         </is>
       </c>
       <c r="C247" s="4" t="inlineStr">
@@ -7102,7 +7159,7 @@
       </c>
       <c r="B248" s="3" t="inlineStr">
         <is>
-          <t>احمد عبدالرحيم عمر بن قاضي</t>
+          <t>مريم احمد عبد المنعم عبد السلام عمار</t>
         </is>
       </c>
       <c r="C248" s="3" t="inlineStr">
@@ -7129,7 +7186,7 @@
       </c>
       <c r="B249" s="4" t="inlineStr">
         <is>
-          <t>عبد الله يوسف محمد الدهام</t>
+          <t xml:space="preserve">جنه وائل كرم محمد فريد </t>
         </is>
       </c>
       <c r="C249" s="4" t="inlineStr">
@@ -7151,12 +7208,12 @@
     <row r="250">
       <c r="A250" s="3" t="inlineStr">
         <is>
-          <t>211566</t>
+          <t>211599</t>
         </is>
       </c>
       <c r="B250" s="3" t="inlineStr">
         <is>
-          <t>حمزه خالد احمد عبد الله البتول</t>
+          <t>محمد فتح الرحمن محمد عمر</t>
         </is>
       </c>
       <c r="C250" s="3" t="inlineStr">
@@ -7178,12 +7235,12 @@
     <row r="251">
       <c r="A251" s="4" t="inlineStr">
         <is>
-          <t>211618</t>
+          <t>211600</t>
         </is>
       </c>
       <c r="B251" s="4" t="inlineStr">
         <is>
-          <t>محمد فتح الرحمن محمد عمر</t>
+          <t>هيثم همام باسم</t>
         </is>
       </c>
       <c r="C251" s="4" t="inlineStr">
@@ -7205,12 +7262,12 @@
     <row r="252">
       <c r="A252" s="3" t="inlineStr">
         <is>
-          <t>211622</t>
+          <t>211601</t>
         </is>
       </c>
       <c r="B252" s="3" t="inlineStr">
         <is>
-          <t>هيثم همام باسم</t>
+          <t>يوسف نبيل موسى</t>
         </is>
       </c>
       <c r="C252" s="3" t="inlineStr">
@@ -7232,12 +7289,12 @@
     <row r="253">
       <c r="A253" s="4" t="inlineStr">
         <is>
-          <t>211628</t>
+          <t>211602</t>
         </is>
       </c>
       <c r="B253" s="4" t="inlineStr">
         <is>
-          <t>يوسف نبيل موسى</t>
+          <t xml:space="preserve">راشد عاطف منصور العبد اللات </t>
         </is>
       </c>
       <c r="C253" s="4" t="inlineStr">
@@ -7259,12 +7316,12 @@
     <row r="254">
       <c r="A254" s="3" t="inlineStr">
         <is>
-          <t>211629</t>
+          <t>211605</t>
         </is>
       </c>
       <c r="B254" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">راشد عاطف منصور العبد اللات </t>
+          <t>احمد ياسر ابراهيم ابو جمعه</t>
         </is>
       </c>
       <c r="C254" s="3" t="inlineStr">
@@ -7286,12 +7343,12 @@
     <row r="255">
       <c r="A255" s="4" t="inlineStr">
         <is>
-          <t>211630</t>
+          <t>211609</t>
         </is>
       </c>
       <c r="B255" s="4" t="inlineStr">
         <is>
-          <t>احمد ياسر ابراهيم ابو جمعه</t>
+          <t>نشأت حسين قسيم العلاونه</t>
         </is>
       </c>
       <c r="C255" s="4" t="inlineStr">
@@ -7313,12 +7370,12 @@
     <row r="256">
       <c r="A256" s="3" t="inlineStr">
         <is>
-          <t>211634</t>
+          <t>211618</t>
         </is>
       </c>
       <c r="B256" s="3" t="inlineStr">
         <is>
-          <t>نشأت حسين قسيم العلاونه</t>
+          <t>ميار احمد يوسف جرادات</t>
         </is>
       </c>
       <c r="C256" s="3" t="inlineStr">
@@ -7340,12 +7397,12 @@
     <row r="257">
       <c r="A257" s="4" t="inlineStr">
         <is>
-          <t>211642</t>
+          <t>211622</t>
         </is>
       </c>
       <c r="B257" s="4" t="inlineStr">
         <is>
-          <t>ميار احمد يوسف جرادات</t>
+          <t>Mahmoud A.M.Assi</t>
         </is>
       </c>
       <c r="C257" s="4" t="inlineStr">
@@ -7367,12 +7424,12 @@
     <row r="258">
       <c r="A258" s="3" t="inlineStr">
         <is>
-          <t>211646</t>
+          <t>211628</t>
         </is>
       </c>
       <c r="B258" s="3" t="inlineStr">
         <is>
-          <t>Mahmoud A.M.Assi</t>
+          <t>اشريفه اب</t>
         </is>
       </c>
       <c r="C258" s="3" t="inlineStr">
@@ -7394,12 +7451,12 @@
     <row r="259">
       <c r="A259" s="4" t="inlineStr">
         <is>
-          <t>211657</t>
+          <t>211629</t>
         </is>
       </c>
       <c r="B259" s="4" t="inlineStr">
         <is>
-          <t>اشريفه اب</t>
+          <t>رئال خالد صالح</t>
         </is>
       </c>
       <c r="C259" s="4" t="inlineStr">
@@ -7421,12 +7478,12 @@
     <row r="260">
       <c r="A260" s="3" t="inlineStr">
         <is>
-          <t>211659</t>
+          <t>211630</t>
         </is>
       </c>
       <c r="B260" s="3" t="inlineStr">
         <is>
-          <t>رئال خالد صالح</t>
+          <t>بكر عبد الله على وريدات</t>
         </is>
       </c>
       <c r="C260" s="3" t="inlineStr">
@@ -7448,12 +7505,12 @@
     <row r="261">
       <c r="A261" s="4" t="inlineStr">
         <is>
-          <t>211664</t>
+          <t>211634</t>
         </is>
       </c>
       <c r="B261" s="4" t="inlineStr">
         <is>
-          <t>بكر عبد الله على وريدات</t>
+          <t>Ghassan Mohammed Hasan</t>
         </is>
       </c>
       <c r="C261" s="4" t="inlineStr">
@@ -7475,12 +7532,12 @@
     <row r="262">
       <c r="A262" s="3" t="inlineStr">
         <is>
-          <t>211666</t>
+          <t>211642</t>
         </is>
       </c>
       <c r="B262" s="3" t="inlineStr">
         <is>
-          <t>Ghassan Mohammed Hasan</t>
+          <t>محمد صلاح فايز ابو دواس</t>
         </is>
       </c>
       <c r="C262" s="3" t="inlineStr">
@@ -7502,12 +7559,12 @@
     <row r="263">
       <c r="A263" s="4" t="inlineStr">
         <is>
-          <t>211676</t>
+          <t>211646</t>
         </is>
       </c>
       <c r="B263" s="4" t="inlineStr">
         <is>
-          <t>محمد صلاح فايز ابو دواس</t>
+          <t>عبد الحافظ زيد عبد الحافظ ابو رمان</t>
         </is>
       </c>
       <c r="C263" s="4" t="inlineStr">
@@ -7529,12 +7586,12 @@
     <row r="264">
       <c r="A264" s="3" t="inlineStr">
         <is>
-          <t>211677</t>
+          <t>211657</t>
         </is>
       </c>
       <c r="B264" s="3" t="inlineStr">
         <is>
-          <t>عبد الحافظ زيد عبد الحافظ ابو رمان</t>
+          <t xml:space="preserve">احمد بدر الدين </t>
         </is>
       </c>
       <c r="C264" s="3" t="inlineStr">
@@ -7556,12 +7613,12 @@
     <row r="265">
       <c r="A265" s="4" t="inlineStr">
         <is>
-          <t>211678</t>
+          <t>211659</t>
         </is>
       </c>
       <c r="B265" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">احمد بدر الدين </t>
+          <t>ربى الصديق محمد احمد</t>
         </is>
       </c>
       <c r="C265" s="4" t="inlineStr">
@@ -7583,12 +7640,12 @@
     <row r="266">
       <c r="A266" s="3" t="inlineStr">
         <is>
-          <t>211681</t>
+          <t>211664</t>
         </is>
       </c>
       <c r="B266" s="3" t="inlineStr">
         <is>
-          <t>ربى الصديق محمد احمد</t>
+          <t>انغام يوسف محمد عبد الكريم</t>
         </is>
       </c>
       <c r="C266" s="3" t="inlineStr">
@@ -7610,12 +7667,12 @@
     <row r="267">
       <c r="A267" s="4" t="inlineStr">
         <is>
-          <t>211682</t>
+          <t>211666</t>
         </is>
       </c>
       <c r="B267" s="4" t="inlineStr">
         <is>
-          <t>انغام يوسف محمد عبد الكريم</t>
+          <t>احمد عماد عابد عابد</t>
         </is>
       </c>
       <c r="C267" s="4" t="inlineStr">
@@ -7637,12 +7694,12 @@
     <row r="268">
       <c r="A268" s="3" t="inlineStr">
         <is>
-          <t>211683</t>
+          <t>211676</t>
         </is>
       </c>
       <c r="B268" s="3" t="inlineStr">
         <is>
-          <t>احمد عماد عابد عابد</t>
+          <t>عبد المؤمن عبد المنعم محمد السمارنه</t>
         </is>
       </c>
       <c r="C268" s="3" t="inlineStr">
@@ -7664,12 +7721,12 @@
     <row r="269">
       <c r="A269" s="4" t="inlineStr">
         <is>
-          <t>211684</t>
+          <t>211677</t>
         </is>
       </c>
       <c r="B269" s="4" t="inlineStr">
         <is>
-          <t>عبد المؤمن عبد المنعم محمد السمارنه</t>
+          <t>عمر عبد الله عمر حمد</t>
         </is>
       </c>
       <c r="C269" s="4" t="inlineStr">
@@ -7691,12 +7748,12 @@
     <row r="270">
       <c r="A270" s="3" t="inlineStr">
         <is>
-          <t>211695</t>
+          <t>211678</t>
         </is>
       </c>
       <c r="B270" s="3" t="inlineStr">
         <is>
-          <t>عمر عبد الله عمر حمد</t>
+          <t>سند عمار محمد الصمادى</t>
         </is>
       </c>
       <c r="C270" s="3" t="inlineStr">
@@ -7718,12 +7775,12 @@
     <row r="271">
       <c r="A271" s="4" t="inlineStr">
         <is>
-          <t>211703</t>
+          <t>211681</t>
         </is>
       </c>
       <c r="B271" s="4" t="inlineStr">
         <is>
-          <t>سند عمار محمد الصمادى</t>
+          <t>حمزه خالد احمد عبد الله البتول</t>
         </is>
       </c>
       <c r="C271" s="4" t="inlineStr">
@@ -7745,7 +7802,7 @@
     <row r="272">
       <c r="A272" s="3" t="inlineStr">
         <is>
-          <t>211705</t>
+          <t>211682</t>
         </is>
       </c>
       <c r="B272" s="3" t="inlineStr">
@@ -7772,7 +7829,7 @@
     <row r="273">
       <c r="A273" s="4" t="inlineStr">
         <is>
-          <t>211709</t>
+          <t>211683</t>
         </is>
       </c>
       <c r="B273" s="4" t="inlineStr">
@@ -7799,7 +7856,7 @@
     <row r="274">
       <c r="A274" s="3" t="inlineStr">
         <is>
-          <t>211715</t>
+          <t>211684</t>
         </is>
       </c>
       <c r="B274" s="3" t="inlineStr">
@@ -7826,7 +7883,7 @@
     <row r="275">
       <c r="A275" s="4" t="inlineStr">
         <is>
-          <t>211718</t>
+          <t>211695</t>
         </is>
       </c>
       <c r="B275" s="4" t="inlineStr">
@@ -7853,7 +7910,7 @@
     <row r="276">
       <c r="A276" s="3" t="inlineStr">
         <is>
-          <t>211719</t>
+          <t>211703</t>
         </is>
       </c>
       <c r="B276" s="3" t="inlineStr">
@@ -7880,12 +7937,12 @@
     <row r="277">
       <c r="A277" s="4" t="inlineStr">
         <is>
-          <t>211358</t>
+          <t>211566</t>
         </is>
       </c>
       <c r="B277" s="4" t="inlineStr">
         <is>
-          <t>خالد محروس الاطرش</t>
+          <t>Ranim Abdulmonem Alabbas</t>
         </is>
       </c>
       <c r="C277" s="4" t="inlineStr">
@@ -7907,12 +7964,12 @@
     <row r="278">
       <c r="A278" s="3" t="inlineStr">
         <is>
-          <t>211730</t>
+          <t>211705</t>
         </is>
       </c>
       <c r="B278" s="3" t="inlineStr">
         <is>
-          <t>Ranim Abdulmonem Alabbas</t>
+          <t>احمد فخرى محمود عكور</t>
         </is>
       </c>
       <c r="C278" s="3" t="inlineStr">
@@ -7934,12 +7991,12 @@
     <row r="279">
       <c r="A279" s="4" t="inlineStr">
         <is>
-          <t>211731</t>
+          <t>211709</t>
         </is>
       </c>
       <c r="B279" s="4" t="inlineStr">
         <is>
-          <t>احمد فخرى محمود عكور</t>
+          <t>عثمان عبدالعزيز ميرغني علي</t>
         </is>
       </c>
       <c r="C279" s="4" t="inlineStr">
@@ -7961,12 +8018,12 @@
     <row r="280">
       <c r="A280" s="3" t="inlineStr">
         <is>
-          <t>211738</t>
+          <t>211715</t>
         </is>
       </c>
       <c r="B280" s="3" t="inlineStr">
         <is>
-          <t>عثمان عبدالعزيز ميرغني علي</t>
+          <t>Diyaam.Msabra</t>
         </is>
       </c>
       <c r="C280" s="3" t="inlineStr">
@@ -7988,12 +8045,12 @@
     <row r="281">
       <c r="A281" s="4" t="inlineStr">
         <is>
-          <t>211746</t>
+          <t>211718</t>
         </is>
       </c>
       <c r="B281" s="4" t="inlineStr">
         <is>
-          <t>Diyaam.Msabra</t>
+          <t>سلام سمير النصار</t>
         </is>
       </c>
       <c r="C281" s="4" t="inlineStr">
@@ -8015,12 +8072,12 @@
     <row r="282">
       <c r="A282" s="3" t="inlineStr">
         <is>
-          <t>211749</t>
+          <t>211719</t>
         </is>
       </c>
       <c r="B282" s="3" t="inlineStr">
         <is>
-          <t>سلام سمير النصار</t>
+          <t>ريم الشيخ عبد العزيز زمراوى</t>
         </is>
       </c>
       <c r="C282" s="3" t="inlineStr">
@@ -8042,12 +8099,12 @@
     <row r="283">
       <c r="A283" s="4" t="inlineStr">
         <is>
-          <t>211751</t>
+          <t>211721</t>
         </is>
       </c>
       <c r="B283" s="4" t="inlineStr">
         <is>
-          <t>ريم الشيخ عبد العزيز زمراوى</t>
+          <t>محي الدين محمد مازن كشور</t>
         </is>
       </c>
       <c r="C283" s="4" t="inlineStr">
@@ -8069,12 +8126,12 @@
     <row r="284">
       <c r="A284" s="3" t="inlineStr">
         <is>
-          <t>211755</t>
+          <t>211730</t>
         </is>
       </c>
       <c r="B284" s="3" t="inlineStr">
         <is>
-          <t>محي الدين محمد مازن كشور</t>
+          <t>عبد البارى امين على السدعى</t>
         </is>
       </c>
       <c r="C284" s="3" t="inlineStr">
@@ -8096,12 +8153,12 @@
     <row r="285">
       <c r="A285" s="4" t="inlineStr">
         <is>
-          <t>211758</t>
+          <t>211731</t>
         </is>
       </c>
       <c r="B285" s="4" t="inlineStr">
         <is>
-          <t>عبد البارى امين على السدعى</t>
+          <t>فارس يوسف سلمان الصعيدى</t>
         </is>
       </c>
       <c r="C285" s="4" t="inlineStr">
@@ -8123,12 +8180,12 @@
     <row r="286">
       <c r="A286" s="3" t="inlineStr">
         <is>
-          <t>211763</t>
+          <t>211738</t>
         </is>
       </c>
       <c r="B286" s="3" t="inlineStr">
         <is>
-          <t>فارس يوسف سلمان الصعيدى</t>
+          <t>منار محمد اسماعيل النهمى</t>
         </is>
       </c>
       <c r="C286" s="3" t="inlineStr">
@@ -8150,12 +8207,12 @@
     <row r="287">
       <c r="A287" s="4" t="inlineStr">
         <is>
-          <t>211768</t>
+          <t>211746</t>
         </is>
       </c>
       <c r="B287" s="4" t="inlineStr">
         <is>
-          <t>منار محمد اسماعيل النهمى</t>
+          <t>عبد الرحمن ماجد على السدعى</t>
         </is>
       </c>
       <c r="C287" s="4" t="inlineStr">
@@ -8177,12 +8234,12 @@
     <row r="288">
       <c r="A288" s="3" t="inlineStr">
         <is>
-          <t>211770</t>
+          <t>211749</t>
         </is>
       </c>
       <c r="B288" s="3" t="inlineStr">
         <is>
-          <t>عبد الرحمن ماجد على السدعى</t>
+          <t>هاجر احمد محمد جابر</t>
         </is>
       </c>
       <c r="C288" s="3" t="inlineStr">
@@ -8204,12 +8261,12 @@
     <row r="289">
       <c r="A289" s="4" t="inlineStr">
         <is>
-          <t>211772</t>
+          <t>211751</t>
         </is>
       </c>
       <c r="B289" s="4" t="inlineStr">
         <is>
-          <t>هاجر احمد محمد جابر</t>
+          <t>Besher Emad Nashed</t>
         </is>
       </c>
       <c r="C289" s="4" t="inlineStr">
@@ -8231,12 +8288,12 @@
     <row r="290">
       <c r="A290" s="3" t="inlineStr">
         <is>
-          <t>211773</t>
+          <t>211755</t>
         </is>
       </c>
       <c r="B290" s="3" t="inlineStr">
         <is>
-          <t>Besher Emad Nashed</t>
+          <t>محمد اسماعيل كمال ابو حسنين</t>
         </is>
       </c>
       <c r="C290" s="3" t="inlineStr">
@@ -8258,12 +8315,12 @@
     <row r="291">
       <c r="A291" s="4" t="inlineStr">
         <is>
-          <t>211778</t>
+          <t>211758</t>
         </is>
       </c>
       <c r="B291" s="4" t="inlineStr">
         <is>
-          <t>محمد اسماعيل كمال ابو حسنين</t>
+          <t>راما صالح اعقيل</t>
         </is>
       </c>
       <c r="C291" s="4" t="inlineStr">
@@ -8285,12 +8342,12 @@
     <row r="292">
       <c r="A292" s="3" t="inlineStr">
         <is>
-          <t>211782</t>
+          <t>211763</t>
         </is>
       </c>
       <c r="B292" s="3" t="inlineStr">
         <is>
-          <t>راما صالح اعقيل</t>
+          <t>يوسف مروان محمد هليل</t>
         </is>
       </c>
       <c r="C292" s="3" t="inlineStr">
@@ -8312,12 +8369,12 @@
     <row r="293">
       <c r="A293" s="4" t="inlineStr">
         <is>
-          <t>211784</t>
+          <t>211768</t>
         </is>
       </c>
       <c r="B293" s="4" t="inlineStr">
         <is>
-          <t>يوسف مروان محمد هليل</t>
+          <t>روزيت جبريهويت هايل</t>
         </is>
       </c>
       <c r="C293" s="4" t="inlineStr">
@@ -8339,12 +8396,12 @@
     <row r="294">
       <c r="A294" s="3" t="inlineStr">
         <is>
-          <t>211792</t>
+          <t>211770</t>
         </is>
       </c>
       <c r="B294" s="3" t="inlineStr">
         <is>
-          <t>روزيت جبريهويت هايل</t>
+          <t>ليان فيصل قاسم الكثيرى</t>
         </is>
       </c>
       <c r="C294" s="3" t="inlineStr">
@@ -8366,12 +8423,12 @@
     <row r="295">
       <c r="A295" s="4" t="inlineStr">
         <is>
-          <t>211803</t>
+          <t>211772</t>
         </is>
       </c>
       <c r="B295" s="4" t="inlineStr">
         <is>
-          <t>ليان فيصل قاسم الكثيرى</t>
+          <t>لين اسامه عباس على</t>
         </is>
       </c>
       <c r="C295" s="4" t="inlineStr">
@@ -8393,12 +8450,12 @@
     <row r="296">
       <c r="A296" s="3" t="inlineStr">
         <is>
-          <t>211805</t>
+          <t>211773</t>
         </is>
       </c>
       <c r="B296" s="3" t="inlineStr">
         <is>
-          <t>لين اسامه عباس على</t>
+          <t>دارين نبيل محمود شلالده</t>
         </is>
       </c>
       <c r="C296" s="3" t="inlineStr">
@@ -8420,12 +8477,12 @@
     <row r="297">
       <c r="A297" s="4" t="inlineStr">
         <is>
-          <t>211810</t>
+          <t>211778</t>
         </is>
       </c>
       <c r="B297" s="4" t="inlineStr">
         <is>
-          <t>دارين نبيل محمود شلالده</t>
+          <t>خوله احمد حسن منصور حسن</t>
         </is>
       </c>
       <c r="C297" s="4" t="inlineStr">
@@ -8447,12 +8504,12 @@
     <row r="298">
       <c r="A298" s="3" t="inlineStr">
         <is>
-          <t>211813</t>
+          <t>211782</t>
         </is>
       </c>
       <c r="B298" s="3" t="inlineStr">
         <is>
-          <t>خوله احمد حسن منصور حسن</t>
+          <t>محمد فتح الرحمن عباس الجلقنى</t>
         </is>
       </c>
       <c r="C298" s="3" t="inlineStr">
@@ -8474,12 +8531,12 @@
     <row r="299">
       <c r="A299" s="4" t="inlineStr">
         <is>
-          <t>211815</t>
+          <t>211784</t>
         </is>
       </c>
       <c r="B299" s="4" t="inlineStr">
         <is>
-          <t>احمد اسماعيل محمد بري</t>
+          <t>خالد محروس الاطرش</t>
         </is>
       </c>
       <c r="C299" s="4" t="inlineStr">
@@ -8501,12 +8558,12 @@
     <row r="300">
       <c r="A300" s="3" t="inlineStr">
         <is>
-          <t>211821</t>
+          <t>211792</t>
         </is>
       </c>
       <c r="B300" s="3" t="inlineStr">
         <is>
-          <t>محمد عمر محمود</t>
+          <t>احمد اسماعيل محمد بري</t>
         </is>
       </c>
       <c r="C300" s="3" t="inlineStr">
@@ -8528,12 +8585,12 @@
     <row r="301">
       <c r="A301" s="4" t="inlineStr">
         <is>
-          <t>211826</t>
+          <t>211803</t>
         </is>
       </c>
       <c r="B301" s="4" t="inlineStr">
         <is>
-          <t>نعيمه فارح ورسمى</t>
+          <t>محمد عمر محمود</t>
         </is>
       </c>
       <c r="C301" s="4" t="inlineStr">
@@ -8555,12 +8612,12 @@
     <row r="302">
       <c r="A302" s="3" t="inlineStr">
         <is>
-          <t>211827</t>
+          <t>211805</t>
         </is>
       </c>
       <c r="B302" s="3" t="inlineStr">
         <is>
-          <t>انس محمد سليمان مصطفى</t>
+          <t>نعيمه فارح ورسمى</t>
         </is>
       </c>
       <c r="C302" s="3" t="inlineStr">
@@ -8582,12 +8639,12 @@
     <row r="303">
       <c r="A303" s="4" t="inlineStr">
         <is>
-          <t>211829</t>
+          <t>211810</t>
         </is>
       </c>
       <c r="B303" s="4" t="inlineStr">
         <is>
-          <t>معاذ محمد القادرى</t>
+          <t>انس محمد سليمان مصطفى</t>
         </is>
       </c>
       <c r="C303" s="4" t="inlineStr">
@@ -8609,12 +8666,12 @@
     <row r="304">
       <c r="A304" s="3" t="inlineStr">
         <is>
-          <t>211830</t>
+          <t>211813</t>
         </is>
       </c>
       <c r="B304" s="3" t="inlineStr">
         <is>
-          <t>اياد ايمن الشفيع احمد</t>
+          <t>معاذ محمد القادرى</t>
         </is>
       </c>
       <c r="C304" s="3" t="inlineStr">
@@ -8641,7 +8698,7 @@
       </c>
       <c r="B305" s="4" t="inlineStr">
         <is>
-          <t>محمد فتح الرحمن عباس الجلقنى</t>
+          <t>اياد ايمن الشفيع احمد</t>
         </is>
       </c>
       <c r="C305" s="4" t="inlineStr">
@@ -8663,12 +8720,12 @@
     <row r="306">
       <c r="A306" s="3" t="inlineStr">
         <is>
-          <t>210872</t>
+          <t>211358</t>
         </is>
       </c>
       <c r="B306" s="3" t="inlineStr">
         <is>
-          <t>امجاد هانى سالم الجابرى</t>
+          <t>يوسف احمد اسماعيل هانى محمد السراج</t>
         </is>
       </c>
       <c r="C306" s="3" t="inlineStr">
@@ -8690,12 +8747,12 @@
     <row r="307">
       <c r="A307" s="4" t="inlineStr">
         <is>
-          <t>211836</t>
+          <t>211815</t>
         </is>
       </c>
       <c r="B307" s="4" t="inlineStr">
         <is>
-          <t>يوسف احمد اسماعيل هانى محمد السراج</t>
+          <t>Rahaf Ghanem Al Sharou</t>
         </is>
       </c>
       <c r="C307" s="4" t="inlineStr">
@@ -8717,12 +8774,12 @@
     <row r="308">
       <c r="A308" s="3" t="inlineStr">
         <is>
-          <t>211837</t>
+          <t>211821</t>
         </is>
       </c>
       <c r="B308" s="3" t="inlineStr">
         <is>
-          <t>Rahaf Ghanem Al Sharou</t>
+          <t>اويس سلمان محمد حمود</t>
         </is>
       </c>
       <c r="C308" s="3" t="inlineStr">
@@ -8744,12 +8801,12 @@
     <row r="309">
       <c r="A309" s="4" t="inlineStr">
         <is>
-          <t>211838</t>
+          <t>211826</t>
         </is>
       </c>
       <c r="B309" s="4" t="inlineStr">
         <is>
-          <t>اويس سلمان محمد حمود</t>
+          <t>طلال صقر ظاهر الفواز</t>
         </is>
       </c>
       <c r="C309" s="4" t="inlineStr">
@@ -8771,12 +8828,12 @@
     <row r="310">
       <c r="A310" s="3" t="inlineStr">
         <is>
-          <t>211843</t>
+          <t>211827</t>
         </is>
       </c>
       <c r="B310" s="3" t="inlineStr">
         <is>
-          <t>طلال صقر ظاهر الفواز</t>
+          <t>محمد خالد صبح جمعه الزومان</t>
         </is>
       </c>
       <c r="C310" s="3" t="inlineStr">
@@ -8798,12 +8855,12 @@
     <row r="311">
       <c r="A311" s="4" t="inlineStr">
         <is>
-          <t>211845</t>
+          <t>211829</t>
         </is>
       </c>
       <c r="B311" s="4" t="inlineStr">
         <is>
-          <t>محمد خالد صبح جمعه الزومان</t>
+          <t>ملاك صبرى عبد الحكيم ناصر</t>
         </is>
       </c>
       <c r="C311" s="4" t="inlineStr">
@@ -8825,12 +8882,12 @@
     <row r="312">
       <c r="A312" s="3" t="inlineStr">
         <is>
-          <t>211846</t>
+          <t>211830</t>
         </is>
       </c>
       <c r="B312" s="3" t="inlineStr">
         <is>
-          <t>ملاك صبرى عبد الحكيم ناصر</t>
+          <t>Ayman Ali Abdullah Alhaddad</t>
         </is>
       </c>
       <c r="C312" s="3" t="inlineStr">
@@ -8852,12 +8909,12 @@
     <row r="313">
       <c r="A313" s="4" t="inlineStr">
         <is>
-          <t>211847</t>
+          <t>211833</t>
         </is>
       </c>
       <c r="B313" s="4" t="inlineStr">
         <is>
-          <t>Ayman Ali Abdullah Alhaddad</t>
+          <t>عثمان عبد الناصر ليلى</t>
         </is>
       </c>
       <c r="C313" s="4" t="inlineStr">
@@ -8879,12 +8936,12 @@
     <row r="314">
       <c r="A314" s="3" t="inlineStr">
         <is>
-          <t>211849</t>
+          <t>211836</t>
         </is>
       </c>
       <c r="B314" s="3" t="inlineStr">
         <is>
-          <t>عثمان عبد الناصر ليلى</t>
+          <t>محمد النور موسى بكر</t>
         </is>
       </c>
       <c r="C314" s="3" t="inlineStr">
@@ -8906,12 +8963,12 @@
     <row r="315">
       <c r="A315" s="4" t="inlineStr">
         <is>
-          <t>211850</t>
+          <t>211837</t>
         </is>
       </c>
       <c r="B315" s="4" t="inlineStr">
         <is>
-          <t>محمد النور موسى بكر</t>
+          <t>محمود عاصم حسن محمود</t>
         </is>
       </c>
       <c r="C315" s="4" t="inlineStr">
@@ -8933,12 +8990,12 @@
     <row r="316">
       <c r="A316" s="3" t="inlineStr">
         <is>
-          <t>211853</t>
+          <t>211838</t>
         </is>
       </c>
       <c r="B316" s="3" t="inlineStr">
         <is>
-          <t>محمود عاصم حسن محمود</t>
+          <t>امينه نور الدين حناوى</t>
         </is>
       </c>
       <c r="C316" s="3" t="inlineStr">
@@ -8960,12 +9017,12 @@
     <row r="317">
       <c r="A317" s="4" t="inlineStr">
         <is>
-          <t>211857</t>
+          <t>211843</t>
         </is>
       </c>
       <c r="B317" s="4" t="inlineStr">
         <is>
-          <t>امينه نور الدين حناوى</t>
+          <t>خالد وليد على البداوى</t>
         </is>
       </c>
       <c r="C317" s="4" t="inlineStr">
@@ -8987,12 +9044,12 @@
     <row r="318">
       <c r="A318" s="3" t="inlineStr">
         <is>
-          <t>211859</t>
+          <t>211845</t>
         </is>
       </c>
       <c r="B318" s="3" t="inlineStr">
         <is>
-          <t>خالد وليد على البداوى</t>
+          <t>فرح جميل عياش الشباكى</t>
         </is>
       </c>
       <c r="C318" s="3" t="inlineStr">
@@ -9014,12 +9071,12 @@
     <row r="319">
       <c r="A319" s="4" t="inlineStr">
         <is>
-          <t>211871</t>
+          <t>211846</t>
         </is>
       </c>
       <c r="B319" s="4" t="inlineStr">
         <is>
-          <t>فرح جميل عياش الشباكى</t>
+          <t>الياس مجدى محمد صالح</t>
         </is>
       </c>
       <c r="C319" s="4" t="inlineStr">
@@ -9041,12 +9098,12 @@
     <row r="320">
       <c r="A320" s="3" t="inlineStr">
         <is>
-          <t>211909</t>
+          <t>211847</t>
         </is>
       </c>
       <c r="B320" s="3" t="inlineStr">
         <is>
-          <t>الياس مجدى محمد صالح</t>
+          <t>محمد وليد داود متعب طحاينه</t>
         </is>
       </c>
       <c r="C320" s="3" t="inlineStr">
@@ -9068,12 +9125,12 @@
     <row r="321">
       <c r="A321" s="4" t="inlineStr">
         <is>
-          <t>211912</t>
+          <t>211849</t>
         </is>
       </c>
       <c r="B321" s="4" t="inlineStr">
         <is>
-          <t>محمد وليد داود متعب طحاينه</t>
+          <t>محمد سليمان خالد درويش</t>
         </is>
       </c>
       <c r="C321" s="4" t="inlineStr">
@@ -9095,12 +9152,12 @@
     <row r="322">
       <c r="A322" s="3" t="inlineStr">
         <is>
-          <t>211923</t>
+          <t>211850</t>
         </is>
       </c>
       <c r="B322" s="3" t="inlineStr">
         <is>
-          <t>محمد سليمان خالد درويش</t>
+          <t>امجد عبد الفتاح احمد الكامل</t>
         </is>
       </c>
       <c r="C322" s="3" t="inlineStr">
@@ -9122,12 +9179,12 @@
     <row r="323">
       <c r="A323" s="4" t="inlineStr">
         <is>
-          <t>211924</t>
+          <t>211853</t>
         </is>
       </c>
       <c r="B323" s="4" t="inlineStr">
         <is>
-          <t>امجد عبد الفتاح احمد الكامل</t>
+          <t>دانا يعقوب هنرى زيادة</t>
         </is>
       </c>
       <c r="C323" s="4" t="inlineStr">
@@ -9149,12 +9206,12 @@
     <row r="324">
       <c r="A324" s="3" t="inlineStr">
         <is>
-          <t>211927</t>
+          <t>211857</t>
         </is>
       </c>
       <c r="B324" s="3" t="inlineStr">
         <is>
-          <t>دانا يعقوب هنرى زيادة</t>
+          <t>عبد الرحمن امين عبد الكريم صبح</t>
         </is>
       </c>
       <c r="C324" s="3" t="inlineStr">
@@ -9176,12 +9233,12 @@
     <row r="325">
       <c r="A325" s="4" t="inlineStr">
         <is>
-          <t>211928</t>
+          <t>211859</t>
         </is>
       </c>
       <c r="B325" s="4" t="inlineStr">
         <is>
-          <t>عبد الرحمن امين عبد الكريم صبح</t>
+          <t>رضوان امين عبد الكريم صبح</t>
         </is>
       </c>
       <c r="C325" s="4" t="inlineStr">
@@ -9203,12 +9260,12 @@
     <row r="326">
       <c r="A326" s="3" t="inlineStr">
         <is>
-          <t>211929</t>
+          <t>211871</t>
         </is>
       </c>
       <c r="B326" s="3" t="inlineStr">
         <is>
-          <t>رضوان امين عبد الكريم صبح</t>
+          <t>رزان محمد ابراهيم عوده</t>
         </is>
       </c>
       <c r="C326" s="3" t="inlineStr">
@@ -9230,12 +9287,12 @@
     <row r="327">
       <c r="A327" s="4" t="inlineStr">
         <is>
-          <t>211930</t>
+          <t>211909</t>
         </is>
       </c>
       <c r="B327" s="4" t="inlineStr">
         <is>
-          <t>بشرى زكريا قباله</t>
+          <t>عمر وائل عبده حسبو محمد</t>
         </is>
       </c>
       <c r="C327" s="4" t="inlineStr">
@@ -9257,12 +9314,12 @@
     <row r="328">
       <c r="A328" s="3" t="inlineStr">
         <is>
-          <t>211931</t>
+          <t>211912</t>
         </is>
       </c>
       <c r="B328" s="3" t="inlineStr">
         <is>
-          <t>ايه الايادى</t>
+          <t>امجاد هانى سالم الجابرى</t>
         </is>
       </c>
       <c r="C328" s="3" t="inlineStr">
@@ -9284,12 +9341,12 @@
     <row r="329">
       <c r="A329" s="4" t="inlineStr">
         <is>
-          <t>211940</t>
+          <t>211923</t>
         </is>
       </c>
       <c r="B329" s="4" t="inlineStr">
         <is>
-          <t>عبد الله عبد الكريم عبد الله بن هرهره</t>
+          <t>بشرى زكريا قباله</t>
         </is>
       </c>
       <c r="C329" s="4" t="inlineStr">
@@ -9311,12 +9368,12 @@
     <row r="330">
       <c r="A330" s="3" t="inlineStr">
         <is>
-          <t>211942</t>
+          <t>211924</t>
         </is>
       </c>
       <c r="B330" s="3" t="inlineStr">
         <is>
-          <t>محمود عبد الله دهان</t>
+          <t>ايه الايادى</t>
         </is>
       </c>
       <c r="C330" s="3" t="inlineStr">
@@ -9338,12 +9395,12 @@
     <row r="331">
       <c r="A331" s="4" t="inlineStr">
         <is>
-          <t>211943</t>
+          <t>211927</t>
         </is>
       </c>
       <c r="B331" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">الجوهرة ايمن موسى حبيب </t>
+          <t>عبد الله عبد الكريم عبد الله بن هرهره</t>
         </is>
       </c>
       <c r="C331" s="4" t="inlineStr">
@@ -9365,12 +9422,12 @@
     <row r="332">
       <c r="A332" s="3" t="inlineStr">
         <is>
-          <t>211945</t>
+          <t>211928</t>
         </is>
       </c>
       <c r="B332" s="3" t="inlineStr">
         <is>
-          <t>هديل محمد صابر ابو زيتون</t>
+          <t>محمود عبد الله دهان</t>
         </is>
       </c>
       <c r="C332" s="3" t="inlineStr">
@@ -9392,12 +9449,12 @@
     <row r="333">
       <c r="A333" s="4" t="inlineStr">
         <is>
-          <t>211946</t>
+          <t>211929</t>
         </is>
       </c>
       <c r="B333" s="4" t="inlineStr">
         <is>
-          <t>راشده رشاد محمد رشاد ال خطاب</t>
+          <t xml:space="preserve">الجوهرة ايمن موسى حبيب </t>
         </is>
       </c>
       <c r="C333" s="4" t="inlineStr">
@@ -9424,7 +9481,7 @@
       </c>
       <c r="B334" s="3" t="inlineStr">
         <is>
-          <t>رزان محمد ابراهيم عوده</t>
+          <t>هديل محمد صابر ابو زيتون</t>
         </is>
       </c>
       <c r="C334" s="3" t="inlineStr">
@@ -9451,7 +9508,7 @@
       </c>
       <c r="B335" s="4" t="inlineStr">
         <is>
-          <t>عمر وائل عبده حسبو محمد</t>
+          <t>راشده رشاد محمد رشاد ال خطاب</t>
         </is>
       </c>
       <c r="C335" s="4" t="inlineStr">
@@ -9471,6 +9528,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>